<commit_message>
fixed the some of the height number in the skyteks slide tab in excel file
</commit_message>
<xml_diff>
--- a/price-list-main.xlsx
+++ b/price-list-main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\smart pergola\smart-pergola-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5544451E-D0A0-4B23-8B49-ED7B8CE14227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5A871F-CEED-44E9-B5BD-7C728875AB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="846" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="846" firstSheet="16" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1300 STANDARD" sheetId="15" state="hidden" r:id="rId1"/>
@@ -2447,7 +2447,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="16">
+  <numFmts count="17">
     <numFmt numFmtId="164" formatCode="_ &quot;₪&quot;\ * #,##0.00_ ;_ &quot;₪&quot;\ * \-#,##0.00_ ;_ &quot;₪&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="#,##0\ &quot;₺&quot;;[Red]#,##0\ &quot;₺&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0\ [$€-407];[Red]#,##0\ [$€-407]"/>
@@ -2464,6 +2464,7 @@
     <numFmt numFmtId="177" formatCode="0.0;[Red]0.0"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
     <numFmt numFmtId="179" formatCode="#,##0\ \€"/>
+    <numFmt numFmtId="180" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -3338,7 +3339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="382">
+  <cellXfs count="383">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4185,6 +4186,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
@@ -4202,33 +4230,6 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4305,6 +4306,21 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4332,21 +4348,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4371,6 +4372,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4382,12 +4389,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4457,6 +4458,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -22256,68 +22260,68 @@
       <c r="M5" s="217"/>
       <c r="N5" s="217"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="298" t="s">
+      <c r="Q5" s="307" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="298"/>
-      <c r="S5" s="298"/>
+      <c r="R5" s="307"/>
+      <c r="S5" s="307"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="295" t="s">
+      <c r="B6" s="304" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="296"/>
-      <c r="D6" s="296"/>
-      <c r="E6" s="296"/>
-      <c r="F6" s="296"/>
-      <c r="G6" s="296"/>
-      <c r="H6" s="296"/>
-      <c r="I6" s="297"/>
+      <c r="C6" s="305"/>
+      <c r="D6" s="305"/>
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="306"/>
       <c r="J6" s="217"/>
       <c r="K6" s="217"/>
-      <c r="L6" s="295" t="s">
+      <c r="L6" s="304" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="296"/>
-      <c r="N6" s="296"/>
-      <c r="O6" s="296"/>
-      <c r="P6" s="296"/>
-      <c r="Q6" s="296"/>
-      <c r="R6" s="296"/>
-      <c r="S6" s="297"/>
+      <c r="M6" s="305"/>
+      <c r="N6" s="305"/>
+      <c r="O6" s="305"/>
+      <c r="P6" s="305"/>
+      <c r="Q6" s="305"/>
+      <c r="R6" s="305"/>
+      <c r="S6" s="306"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="293" t="s">
+      <c r="A7" s="302" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="294" t="s">
+      <c r="B7" s="303" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="294"/>
-      <c r="D7" s="294"/>
-      <c r="E7" s="294"/>
-      <c r="F7" s="294"/>
-      <c r="G7" s="294"/>
-      <c r="H7" s="294"/>
-      <c r="I7" s="294"/>
+      <c r="C7" s="303"/>
+      <c r="D7" s="303"/>
+      <c r="E7" s="303"/>
+      <c r="F7" s="303"/>
+      <c r="G7" s="303"/>
+      <c r="H7" s="303"/>
+      <c r="I7" s="303"/>
       <c r="J7" s="217"/>
-      <c r="K7" s="293" t="s">
+      <c r="K7" s="302" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="294" t="s">
+      <c r="L7" s="303" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="294"/>
-      <c r="N7" s="294"/>
-      <c r="O7" s="294"/>
-      <c r="P7" s="294"/>
-      <c r="Q7" s="294"/>
-      <c r="R7" s="294"/>
-      <c r="S7" s="294"/>
+      <c r="M7" s="303"/>
+      <c r="N7" s="303"/>
+      <c r="O7" s="303"/>
+      <c r="P7" s="303"/>
+      <c r="Q7" s="303"/>
+      <c r="R7" s="303"/>
+      <c r="S7" s="303"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="293"/>
+      <c r="A8" s="302"/>
       <c r="B8" s="89"/>
       <c r="C8" s="90">
         <v>1750</v>
@@ -22341,7 +22345,7 @@
         <v>3250</v>
       </c>
       <c r="J8" s="217"/>
-      <c r="K8" s="293"/>
+      <c r="K8" s="302"/>
       <c r="L8" s="89"/>
       <c r="M8" s="90">
         <v>1750</v>
@@ -22366,7 +22370,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="293"/>
+      <c r="A9" s="302"/>
       <c r="B9" s="222">
         <v>1000</v>
       </c>
@@ -22392,7 +22396,7 @@
         <v>1785</v>
       </c>
       <c r="J9" s="217"/>
-      <c r="K9" s="293"/>
+      <c r="K9" s="302"/>
       <c r="L9" s="222">
         <v>1000</v>
       </c>
@@ -22419,7 +22423,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="293"/>
+      <c r="A10" s="302"/>
       <c r="B10" s="222">
         <v>1250</v>
       </c>
@@ -22445,7 +22449,7 @@
         <v>1928.5</v>
       </c>
       <c r="J10" s="217"/>
-      <c r="K10" s="293"/>
+      <c r="K10" s="302"/>
       <c r="L10" s="222">
         <v>1250</v>
       </c>
@@ -22472,7 +22476,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="293"/>
+      <c r="A11" s="302"/>
       <c r="B11" s="222">
         <v>1500</v>
       </c>
@@ -22498,7 +22502,7 @@
         <v>2072</v>
       </c>
       <c r="J11" s="217"/>
-      <c r="K11" s="293"/>
+      <c r="K11" s="302"/>
       <c r="L11" s="222">
         <v>1500</v>
       </c>
@@ -22525,7 +22529,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="293"/>
+      <c r="A12" s="302"/>
       <c r="B12" s="222">
         <v>1750</v>
       </c>
@@ -22551,7 +22555,7 @@
         <v>2215.5</v>
       </c>
       <c r="J12" s="217"/>
-      <c r="K12" s="293"/>
+      <c r="K12" s="302"/>
       <c r="L12" s="222">
         <v>1750</v>
       </c>
@@ -22578,7 +22582,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="293"/>
+      <c r="A13" s="302"/>
       <c r="B13" s="222">
         <v>2000</v>
       </c>
@@ -22604,7 +22608,7 @@
         <v>2450</v>
       </c>
       <c r="J13" s="217"/>
-      <c r="K13" s="293"/>
+      <c r="K13" s="302"/>
       <c r="L13" s="222">
         <v>2000</v>
       </c>
@@ -22631,7 +22635,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="293"/>
+      <c r="A14" s="302"/>
       <c r="B14" s="222">
         <v>2250</v>
       </c>
@@ -22657,7 +22661,7 @@
         <v>2593.5</v>
       </c>
       <c r="J14" s="217"/>
-      <c r="K14" s="293"/>
+      <c r="K14" s="302"/>
       <c r="L14" s="222">
         <v>2250</v>
       </c>
@@ -22684,7 +22688,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="293"/>
+      <c r="A15" s="302"/>
       <c r="B15" s="222">
         <v>2500</v>
       </c>
@@ -22710,7 +22714,7 @@
         <v>2740.5</v>
       </c>
       <c r="J15" s="217"/>
-      <c r="K15" s="293"/>
+      <c r="K15" s="302"/>
       <c r="L15" s="222">
         <v>2500</v>
       </c>
@@ -22737,7 +22741,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="293"/>
+      <c r="A16" s="302"/>
       <c r="B16" s="222">
         <v>2750</v>
       </c>
@@ -22763,7 +22767,7 @@
         <v>2884</v>
       </c>
       <c r="J16" s="217"/>
-      <c r="K16" s="293"/>
+      <c r="K16" s="302"/>
       <c r="L16" s="222">
         <v>2750</v>
       </c>
@@ -22790,7 +22794,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="293"/>
+      <c r="A17" s="302"/>
       <c r="B17" s="222">
         <v>3000</v>
       </c>
@@ -22816,7 +22820,7 @@
         <v>3038</v>
       </c>
       <c r="J17" s="217"/>
-      <c r="K17" s="293"/>
+      <c r="K17" s="302"/>
       <c r="L17" s="222">
         <v>3000</v>
       </c>
@@ -22843,7 +22847,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="293"/>
+      <c r="A18" s="302"/>
       <c r="B18" s="222">
         <v>3250</v>
       </c>
@@ -22869,7 +22873,7 @@
         <v>3181.5</v>
       </c>
       <c r="J18" s="217"/>
-      <c r="K18" s="293"/>
+      <c r="K18" s="302"/>
       <c r="L18" s="222">
         <v>3250</v>
       </c>
@@ -22896,7 +22900,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="293"/>
+      <c r="A19" s="302"/>
       <c r="B19" s="222">
         <v>3500</v>
       </c>
@@ -22922,7 +22926,7 @@
         <v>6</v>
       </c>
       <c r="J19" s="217"/>
-      <c r="K19" s="293"/>
+      <c r="K19" s="302"/>
       <c r="L19" s="222">
         <v>3500</v>
       </c>
@@ -22949,7 +22953,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="293"/>
+      <c r="A20" s="302"/>
       <c r="B20" s="222">
         <v>3750</v>
       </c>
@@ -22975,7 +22979,7 @@
         <v>6</v>
       </c>
       <c r="J20" s="217"/>
-      <c r="K20" s="293"/>
+      <c r="K20" s="302"/>
       <c r="L20" s="222">
         <v>3750</v>
       </c>
@@ -23002,7 +23006,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="293"/>
+      <c r="A21" s="302"/>
       <c r="B21" s="222">
         <v>4000</v>
       </c>
@@ -23028,7 +23032,7 @@
         <v>6</v>
       </c>
       <c r="J21" s="217"/>
-      <c r="K21" s="293"/>
+      <c r="K21" s="302"/>
       <c r="L21" s="222">
         <v>4000</v>
       </c>
@@ -23103,125 +23107,125 @@
     </row>
     <row r="25" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="299" t="s">
+      <c r="B25" s="295" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="299"/>
-      <c r="D25" s="299"/>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
-      <c r="G25" s="299"/>
-      <c r="H25" s="299"/>
+      <c r="C25" s="295"/>
+      <c r="D25" s="295"/>
+      <c r="E25" s="295"/>
+      <c r="F25" s="295"/>
+      <c r="G25" s="295"/>
+      <c r="H25" s="295"/>
       <c r="I25" s="217"/>
       <c r="J25" s="217"/>
       <c r="K25" s="217"/>
-      <c r="L25" s="299" t="s">
+      <c r="L25" s="295" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="299"/>
-      <c r="N25" s="299"/>
-      <c r="O25" s="299"/>
-      <c r="P25" s="299"/>
-      <c r="Q25" s="299"/>
-      <c r="R25" s="299"/>
+      <c r="M25" s="295"/>
+      <c r="N25" s="295"/>
+      <c r="O25" s="295"/>
+      <c r="P25" s="295"/>
+      <c r="Q25" s="295"/>
+      <c r="R25" s="295"/>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="300" t="s">
+      <c r="B26" s="296" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="300"/>
-      <c r="D26" s="300"/>
-      <c r="E26" s="300"/>
-      <c r="F26" s="302">
+      <c r="C26" s="296"/>
+      <c r="D26" s="296"/>
+      <c r="E26" s="296"/>
+      <c r="F26" s="299">
         <v>88</v>
       </c>
-      <c r="G26" s="303"/>
-      <c r="H26" s="303"/>
+      <c r="G26" s="300"/>
+      <c r="H26" s="300"/>
       <c r="I26" s="217"/>
       <c r="J26" s="217"/>
       <c r="K26" s="217"/>
-      <c r="L26" s="300" t="s">
+      <c r="L26" s="296" t="s">
         <v>77</v>
       </c>
-      <c r="M26" s="300"/>
-      <c r="N26" s="306" t="s">
+      <c r="M26" s="296"/>
+      <c r="N26" s="297" t="s">
         <v>78</v>
       </c>
-      <c r="O26" s="306"/>
-      <c r="P26" s="306"/>
-      <c r="Q26" s="306"/>
-      <c r="R26" s="306"/>
+      <c r="O26" s="297"/>
+      <c r="P26" s="297"/>
+      <c r="Q26" s="297"/>
+      <c r="R26" s="297"/>
     </row>
     <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="301" t="s">
+      <c r="B27" s="293" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="301"/>
-      <c r="D27" s="301"/>
-      <c r="E27" s="301"/>
-      <c r="F27" s="302">
+      <c r="C27" s="293"/>
+      <c r="D27" s="293"/>
+      <c r="E27" s="293"/>
+      <c r="F27" s="299">
         <v>132</v>
       </c>
-      <c r="G27" s="303"/>
-      <c r="H27" s="303"/>
+      <c r="G27" s="300"/>
+      <c r="H27" s="300"/>
       <c r="I27" s="217"/>
       <c r="J27" s="217"/>
       <c r="K27" s="217"/>
-      <c r="L27" s="301" t="s">
+      <c r="L27" s="293" t="s">
         <v>80</v>
       </c>
-      <c r="M27" s="301"/>
-      <c r="N27" s="305" t="s">
+      <c r="M27" s="293"/>
+      <c r="N27" s="294" t="s">
         <v>81</v>
       </c>
-      <c r="O27" s="305"/>
-      <c r="P27" s="305"/>
-      <c r="Q27" s="305"/>
-      <c r="R27" s="305"/>
+      <c r="O27" s="294"/>
+      <c r="P27" s="294"/>
+      <c r="Q27" s="294"/>
+      <c r="R27" s="294"/>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="301" t="s">
+      <c r="B28" s="293" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="301"/>
-      <c r="D28" s="301"/>
-      <c r="E28" s="301"/>
-      <c r="F28" s="302">
+      <c r="C28" s="293"/>
+      <c r="D28" s="293"/>
+      <c r="E28" s="293"/>
+      <c r="F28" s="299">
         <v>229</v>
       </c>
-      <c r="G28" s="303"/>
-      <c r="H28" s="303"/>
+      <c r="G28" s="300"/>
+      <c r="H28" s="300"/>
       <c r="I28" s="217"/>
       <c r="J28" s="217"/>
       <c r="K28" s="217"/>
-      <c r="L28" s="301" t="s">
+      <c r="L28" s="293" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="301"/>
-      <c r="N28" s="307" t="s">
+      <c r="M28" s="293"/>
+      <c r="N28" s="298" t="s">
         <v>84</v>
       </c>
-      <c r="O28" s="307"/>
-      <c r="P28" s="307"/>
-      <c r="Q28" s="307"/>
-      <c r="R28" s="307"/>
+      <c r="O28" s="298"/>
+      <c r="P28" s="298"/>
+      <c r="Q28" s="298"/>
+      <c r="R28" s="298"/>
     </row>
     <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="301" t="s">
+      <c r="B29" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="301"/>
-      <c r="D29" s="301"/>
-      <c r="E29" s="301"/>
-      <c r="F29" s="304">
+      <c r="C29" s="293"/>
+      <c r="D29" s="293"/>
+      <c r="E29" s="293"/>
+      <c r="F29" s="301">
         <v>0.03</v>
       </c>
-      <c r="G29" s="304"/>
-      <c r="H29" s="304"/>
+      <c r="G29" s="301"/>
+      <c r="H29" s="301"/>
       <c r="I29" s="217"/>
       <c r="J29" s="217"/>
       <c r="K29" s="217"/>
@@ -23229,83 +23233,83 @@
         <v>86</v>
       </c>
       <c r="M29" s="37"/>
-      <c r="N29" s="305" t="s">
+      <c r="N29" s="294" t="s">
         <v>87</v>
       </c>
-      <c r="O29" s="305"/>
-      <c r="P29" s="305"/>
-      <c r="Q29" s="305"/>
-      <c r="R29" s="305"/>
+      <c r="O29" s="294"/>
+      <c r="P29" s="294"/>
+      <c r="Q29" s="294"/>
+      <c r="R29" s="294"/>
     </row>
     <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="301" t="s">
+      <c r="B30" s="293" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="301"/>
-      <c r="D30" s="301"/>
-      <c r="E30" s="301"/>
-      <c r="F30" s="304">
+      <c r="C30" s="293"/>
+      <c r="D30" s="293"/>
+      <c r="E30" s="293"/>
+      <c r="F30" s="301">
         <v>0.08</v>
       </c>
-      <c r="G30" s="304"/>
-      <c r="H30" s="304"/>
+      <c r="G30" s="301"/>
+      <c r="H30" s="301"/>
       <c r="I30" s="217"/>
       <c r="J30" s="217"/>
       <c r="K30" s="217"/>
-      <c r="L30" s="301" t="s">
+      <c r="L30" s="293" t="s">
         <v>89</v>
       </c>
-      <c r="M30" s="301"/>
-      <c r="N30" s="305" t="s">
+      <c r="M30" s="293"/>
+      <c r="N30" s="294" t="s">
         <v>90</v>
       </c>
-      <c r="O30" s="305"/>
-      <c r="P30" s="305"/>
-      <c r="Q30" s="305"/>
-      <c r="R30" s="305"/>
+      <c r="O30" s="294"/>
+      <c r="P30" s="294"/>
+      <c r="Q30" s="294"/>
+      <c r="R30" s="294"/>
     </row>
     <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="301" t="s">
+      <c r="B31" s="293" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="301"/>
-      <c r="D31" s="301"/>
-      <c r="E31" s="301"/>
-      <c r="F31" s="302">
+      <c r="C31" s="293"/>
+      <c r="D31" s="293"/>
+      <c r="E31" s="293"/>
+      <c r="F31" s="299">
         <v>47</v>
       </c>
-      <c r="G31" s="303"/>
-      <c r="H31" s="303"/>
+      <c r="G31" s="300"/>
+      <c r="H31" s="300"/>
       <c r="I31" s="217"/>
       <c r="J31" s="217"/>
       <c r="K31" s="217"/>
-      <c r="L31" s="301" t="s">
+      <c r="L31" s="293" t="s">
         <v>92</v>
       </c>
-      <c r="M31" s="301"/>
-      <c r="N31" s="305" t="s">
+      <c r="M31" s="293"/>
+      <c r="N31" s="294" t="s">
         <v>93</v>
       </c>
-      <c r="O31" s="305"/>
-      <c r="P31" s="305"/>
-      <c r="Q31" s="305"/>
-      <c r="R31" s="305"/>
+      <c r="O31" s="294"/>
+      <c r="P31" s="294"/>
+      <c r="Q31" s="294"/>
+      <c r="R31" s="294"/>
     </row>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="301" t="s">
+      <c r="B32" s="293" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="301"/>
-      <c r="D32" s="301"/>
-      <c r="E32" s="301"/>
-      <c r="F32" s="302">
+      <c r="C32" s="293"/>
+      <c r="D32" s="293"/>
+      <c r="E32" s="293"/>
+      <c r="F32" s="299">
         <v>10</v>
       </c>
-      <c r="G32" s="303"/>
-      <c r="H32" s="303"/>
+      <c r="G32" s="300"/>
+      <c r="H32" s="300"/>
       <c r="I32" s="217"/>
       <c r="J32" s="217"/>
       <c r="K32" s="217"/>
@@ -23454,6 +23458,35 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="K7:K21"/>
+    <mergeCell ref="L7:S7"/>
+    <mergeCell ref="A7:A21"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="Q1:S4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="L6:S6"/>
+    <mergeCell ref="F1:O4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="P35:S38"/>
+    <mergeCell ref="K35:N38"/>
+    <mergeCell ref="F35:I38"/>
+    <mergeCell ref="A35:D38"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:H32"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="N31:R31"/>
     <mergeCell ref="L25:R25"/>
@@ -23466,35 +23499,6 @@
     <mergeCell ref="N29:R29"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="N30:R30"/>
-    <mergeCell ref="P35:S38"/>
-    <mergeCell ref="K35:N38"/>
-    <mergeCell ref="F35:I38"/>
-    <mergeCell ref="A35:D38"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="K7:K21"/>
-    <mergeCell ref="L7:S7"/>
-    <mergeCell ref="A7:A21"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="Q1:S4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="L6:S6"/>
-    <mergeCell ref="F1:O4"/>
-    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="3.937007874015748E-2" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -23506,7 +23510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C847868E-31B6-467F-A8CD-BA5FFFAD6A65}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -24272,11 +24276,11 @@
       <c r="M5" s="217"/>
       <c r="N5" s="217"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="298" t="s">
+      <c r="Q5" s="307" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="298"/>
-      <c r="S5" s="298"/>
+      <c r="R5" s="307"/>
+      <c r="S5" s="307"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -24292,48 +24296,48 @@
       <c r="I6" s="109"/>
       <c r="J6" s="217"/>
       <c r="K6" s="217"/>
-      <c r="L6" s="295" t="s">
+      <c r="L6" s="304" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="296"/>
-      <c r="N6" s="296"/>
-      <c r="O6" s="296"/>
-      <c r="P6" s="296"/>
-      <c r="Q6" s="296"/>
-      <c r="R6" s="296"/>
-      <c r="S6" s="297"/>
+      <c r="M6" s="305"/>
+      <c r="N6" s="305"/>
+      <c r="O6" s="305"/>
+      <c r="P6" s="305"/>
+      <c r="Q6" s="305"/>
+      <c r="R6" s="305"/>
+      <c r="S6" s="306"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="293" t="s">
+      <c r="A7" s="302" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="294" t="s">
+      <c r="B7" s="303" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="294"/>
-      <c r="D7" s="294"/>
-      <c r="E7" s="294"/>
-      <c r="F7" s="294"/>
-      <c r="G7" s="294"/>
-      <c r="H7" s="294"/>
-      <c r="I7" s="294"/>
+      <c r="C7" s="303"/>
+      <c r="D7" s="303"/>
+      <c r="E7" s="303"/>
+      <c r="F7" s="303"/>
+      <c r="G7" s="303"/>
+      <c r="H7" s="303"/>
+      <c r="I7" s="303"/>
       <c r="J7" s="217"/>
-      <c r="K7" s="293" t="s">
+      <c r="K7" s="302" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="294" t="s">
+      <c r="L7" s="303" t="s">
         <v>71</v>
       </c>
-      <c r="M7" s="294"/>
-      <c r="N7" s="294"/>
-      <c r="O7" s="294"/>
-      <c r="P7" s="294"/>
-      <c r="Q7" s="294"/>
-      <c r="R7" s="294"/>
-      <c r="S7" s="294"/>
+      <c r="M7" s="303"/>
+      <c r="N7" s="303"/>
+      <c r="O7" s="303"/>
+      <c r="P7" s="303"/>
+      <c r="Q7" s="303"/>
+      <c r="R7" s="303"/>
+      <c r="S7" s="303"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="293"/>
+      <c r="A8" s="302"/>
       <c r="B8" s="89"/>
       <c r="C8" s="90">
         <v>1750</v>
@@ -24357,7 +24361,7 @@
         <v>3250</v>
       </c>
       <c r="J8" s="217"/>
-      <c r="K8" s="293"/>
+      <c r="K8" s="302"/>
       <c r="L8" s="89"/>
       <c r="M8" s="90">
         <v>1750</v>
@@ -24382,7 +24386,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="293"/>
+      <c r="A9" s="302"/>
       <c r="B9" s="222">
         <v>1000</v>
       </c>
@@ -24408,7 +24412,7 @@
         <v>1792</v>
       </c>
       <c r="J9" s="217"/>
-      <c r="K9" s="293"/>
+      <c r="K9" s="302"/>
       <c r="L9" s="222">
         <v>1000</v>
       </c>
@@ -24435,7 +24439,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="293"/>
+      <c r="A10" s="302"/>
       <c r="B10" s="222">
         <v>1250</v>
       </c>
@@ -24461,7 +24465,7 @@
         <v>1946</v>
       </c>
       <c r="J10" s="217"/>
-      <c r="K10" s="293"/>
+      <c r="K10" s="302"/>
       <c r="L10" s="222">
         <v>1250</v>
       </c>
@@ -24488,7 +24492,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="293"/>
+      <c r="A11" s="302"/>
       <c r="B11" s="222">
         <v>1500</v>
       </c>
@@ -24514,7 +24518,7 @@
         <v>2100</v>
       </c>
       <c r="J11" s="217"/>
-      <c r="K11" s="293"/>
+      <c r="K11" s="302"/>
       <c r="L11" s="222">
         <v>1500</v>
       </c>
@@ -24541,7 +24545,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="293"/>
+      <c r="A12" s="302"/>
       <c r="B12" s="222">
         <v>1750</v>
       </c>
@@ -24567,7 +24571,7 @@
         <v>2254</v>
       </c>
       <c r="J12" s="217"/>
-      <c r="K12" s="293"/>
+      <c r="K12" s="302"/>
       <c r="L12" s="222">
         <v>1750</v>
       </c>
@@ -24594,7 +24598,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="293"/>
+      <c r="A13" s="302"/>
       <c r="B13" s="222">
         <v>2000</v>
       </c>
@@ -24620,7 +24624,7 @@
         <v>2502.5</v>
       </c>
       <c r="J13" s="217"/>
-      <c r="K13" s="293"/>
+      <c r="K13" s="302"/>
       <c r="L13" s="222">
         <v>2000</v>
       </c>
@@ -24647,7 +24651,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="293"/>
+      <c r="A14" s="302"/>
       <c r="B14" s="222">
         <v>2250</v>
       </c>
@@ -24673,7 +24677,7 @@
         <v>2656.5</v>
       </c>
       <c r="J14" s="217"/>
-      <c r="K14" s="293"/>
+      <c r="K14" s="302"/>
       <c r="L14" s="222">
         <v>2250</v>
       </c>
@@ -24700,7 +24704,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="293"/>
+      <c r="A15" s="302"/>
       <c r="B15" s="222">
         <v>2500</v>
       </c>
@@ -24726,7 +24730,7 @@
         <v>2810.5</v>
       </c>
       <c r="J15" s="217"/>
-      <c r="K15" s="293"/>
+      <c r="K15" s="302"/>
       <c r="L15" s="222">
         <v>2500</v>
       </c>
@@ -24753,7 +24757,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="293"/>
+      <c r="A16" s="302"/>
       <c r="B16" s="222">
         <v>2750</v>
       </c>
@@ -24779,7 +24783,7 @@
         <v>2968</v>
       </c>
       <c r="J16" s="217"/>
-      <c r="K16" s="293"/>
+      <c r="K16" s="302"/>
       <c r="L16" s="222">
         <v>2750</v>
       </c>
@@ -24806,7 +24810,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="293"/>
+      <c r="A17" s="302"/>
       <c r="B17" s="222">
         <v>3000</v>
       </c>
@@ -24832,7 +24836,7 @@
         <v>3132.5</v>
       </c>
       <c r="J17" s="217"/>
-      <c r="K17" s="293"/>
+      <c r="K17" s="302"/>
       <c r="L17" s="222">
         <v>3000</v>
       </c>
@@ -24859,7 +24863,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="293"/>
+      <c r="A18" s="302"/>
       <c r="B18" s="222">
         <v>3250</v>
       </c>
@@ -24885,7 +24889,7 @@
         <v>3286.5</v>
       </c>
       <c r="J18" s="217"/>
-      <c r="K18" s="293"/>
+      <c r="K18" s="302"/>
       <c r="L18" s="222">
         <v>3250</v>
       </c>
@@ -24912,7 +24916,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="293"/>
+      <c r="A19" s="302"/>
       <c r="B19" s="222">
         <v>3500</v>
       </c>
@@ -24938,7 +24942,7 @@
         <v>6</v>
       </c>
       <c r="J19" s="217"/>
-      <c r="K19" s="293"/>
+      <c r="K19" s="302"/>
       <c r="L19" s="222">
         <v>3500</v>
       </c>
@@ -24965,7 +24969,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="293"/>
+      <c r="A20" s="302"/>
       <c r="B20" s="222">
         <v>3750</v>
       </c>
@@ -24991,7 +24995,7 @@
         <v>6</v>
       </c>
       <c r="J20" s="217"/>
-      <c r="K20" s="293"/>
+      <c r="K20" s="302"/>
       <c r="L20" s="222">
         <v>3750</v>
       </c>
@@ -25018,7 +25022,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="293"/>
+      <c r="A21" s="302"/>
       <c r="B21" s="222">
         <v>4000</v>
       </c>
@@ -25044,7 +25048,7 @@
         <v>6</v>
       </c>
       <c r="J21" s="217"/>
-      <c r="K21" s="293"/>
+      <c r="K21" s="302"/>
       <c r="L21" s="222">
         <v>4000</v>
       </c>
@@ -25119,125 +25123,125 @@
     </row>
     <row r="25" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="299" t="s">
+      <c r="B25" s="295" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="299"/>
-      <c r="D25" s="299"/>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
-      <c r="G25" s="299"/>
-      <c r="H25" s="299"/>
+      <c r="C25" s="295"/>
+      <c r="D25" s="295"/>
+      <c r="E25" s="295"/>
+      <c r="F25" s="295"/>
+      <c r="G25" s="295"/>
+      <c r="H25" s="295"/>
       <c r="I25" s="217"/>
       <c r="J25" s="217"/>
       <c r="K25" s="217"/>
-      <c r="L25" s="299" t="s">
+      <c r="L25" s="295" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="299"/>
-      <c r="N25" s="299"/>
-      <c r="O25" s="299"/>
-      <c r="P25" s="299"/>
-      <c r="Q25" s="299"/>
-      <c r="R25" s="299"/>
+      <c r="M25" s="295"/>
+      <c r="N25" s="295"/>
+      <c r="O25" s="295"/>
+      <c r="P25" s="295"/>
+      <c r="Q25" s="295"/>
+      <c r="R25" s="295"/>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="300" t="s">
+      <c r="B26" s="296" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="300"/>
-      <c r="D26" s="300"/>
-      <c r="E26" s="300"/>
-      <c r="F26" s="302">
+      <c r="C26" s="296"/>
+      <c r="D26" s="296"/>
+      <c r="E26" s="296"/>
+      <c r="F26" s="299">
         <v>88</v>
       </c>
-      <c r="G26" s="303"/>
-      <c r="H26" s="303"/>
+      <c r="G26" s="300"/>
+      <c r="H26" s="300"/>
       <c r="I26" s="217"/>
       <c r="J26" s="217"/>
       <c r="K26" s="217"/>
-      <c r="L26" s="300" t="s">
+      <c r="L26" s="296" t="s">
         <v>77</v>
       </c>
-      <c r="M26" s="300"/>
-      <c r="N26" s="306" t="s">
+      <c r="M26" s="296"/>
+      <c r="N26" s="297" t="s">
         <v>78</v>
       </c>
-      <c r="O26" s="306"/>
-      <c r="P26" s="306"/>
-      <c r="Q26" s="306"/>
-      <c r="R26" s="306"/>
+      <c r="O26" s="297"/>
+      <c r="P26" s="297"/>
+      <c r="Q26" s="297"/>
+      <c r="R26" s="297"/>
     </row>
     <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="301" t="s">
+      <c r="B27" s="293" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="301"/>
-      <c r="D27" s="301"/>
-      <c r="E27" s="301"/>
-      <c r="F27" s="302">
+      <c r="C27" s="293"/>
+      <c r="D27" s="293"/>
+      <c r="E27" s="293"/>
+      <c r="F27" s="299">
         <v>132</v>
       </c>
-      <c r="G27" s="303"/>
-      <c r="H27" s="303"/>
+      <c r="G27" s="300"/>
+      <c r="H27" s="300"/>
       <c r="I27" s="217"/>
       <c r="J27" s="217"/>
       <c r="K27" s="217"/>
-      <c r="L27" s="301" t="s">
+      <c r="L27" s="293" t="s">
         <v>80</v>
       </c>
-      <c r="M27" s="301"/>
-      <c r="N27" s="305" t="s">
+      <c r="M27" s="293"/>
+      <c r="N27" s="294" t="s">
         <v>81</v>
       </c>
-      <c r="O27" s="305"/>
-      <c r="P27" s="305"/>
-      <c r="Q27" s="305"/>
-      <c r="R27" s="305"/>
+      <c r="O27" s="294"/>
+      <c r="P27" s="294"/>
+      <c r="Q27" s="294"/>
+      <c r="R27" s="294"/>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="301" t="s">
+      <c r="B28" s="293" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="301"/>
-      <c r="D28" s="301"/>
-      <c r="E28" s="301"/>
-      <c r="F28" s="302">
+      <c r="C28" s="293"/>
+      <c r="D28" s="293"/>
+      <c r="E28" s="293"/>
+      <c r="F28" s="299">
         <v>229</v>
       </c>
-      <c r="G28" s="303"/>
-      <c r="H28" s="303"/>
+      <c r="G28" s="300"/>
+      <c r="H28" s="300"/>
       <c r="I28" s="217"/>
       <c r="J28" s="217"/>
       <c r="K28" s="217"/>
-      <c r="L28" s="301" t="s">
+      <c r="L28" s="293" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="301"/>
-      <c r="N28" s="307" t="s">
+      <c r="M28" s="293"/>
+      <c r="N28" s="298" t="s">
         <v>84</v>
       </c>
-      <c r="O28" s="307"/>
-      <c r="P28" s="307"/>
-      <c r="Q28" s="307"/>
-      <c r="R28" s="307"/>
+      <c r="O28" s="298"/>
+      <c r="P28" s="298"/>
+      <c r="Q28" s="298"/>
+      <c r="R28" s="298"/>
     </row>
     <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="301" t="s">
+      <c r="B29" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="301"/>
-      <c r="D29" s="301"/>
-      <c r="E29" s="301"/>
-      <c r="F29" s="304">
+      <c r="C29" s="293"/>
+      <c r="D29" s="293"/>
+      <c r="E29" s="293"/>
+      <c r="F29" s="301">
         <v>0.03</v>
       </c>
-      <c r="G29" s="304"/>
-      <c r="H29" s="304"/>
+      <c r="G29" s="301"/>
+      <c r="H29" s="301"/>
       <c r="I29" s="217"/>
       <c r="J29" s="217"/>
       <c r="K29" s="217"/>
@@ -25245,83 +25249,83 @@
         <v>86</v>
       </c>
       <c r="M29" s="37"/>
-      <c r="N29" s="305" t="s">
+      <c r="N29" s="294" t="s">
         <v>87</v>
       </c>
-      <c r="O29" s="305"/>
-      <c r="P29" s="305"/>
-      <c r="Q29" s="305"/>
-      <c r="R29" s="305"/>
+      <c r="O29" s="294"/>
+      <c r="P29" s="294"/>
+      <c r="Q29" s="294"/>
+      <c r="R29" s="294"/>
     </row>
     <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="301" t="s">
+      <c r="B30" s="293" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="301"/>
-      <c r="D30" s="301"/>
-      <c r="E30" s="301"/>
-      <c r="F30" s="304">
+      <c r="C30" s="293"/>
+      <c r="D30" s="293"/>
+      <c r="E30" s="293"/>
+      <c r="F30" s="301">
         <v>0.08</v>
       </c>
-      <c r="G30" s="304"/>
-      <c r="H30" s="304"/>
+      <c r="G30" s="301"/>
+      <c r="H30" s="301"/>
       <c r="I30" s="217"/>
       <c r="J30" s="217"/>
       <c r="K30" s="217"/>
-      <c r="L30" s="301" t="s">
+      <c r="L30" s="293" t="s">
         <v>89</v>
       </c>
-      <c r="M30" s="301"/>
-      <c r="N30" s="305" t="s">
+      <c r="M30" s="293"/>
+      <c r="N30" s="294" t="s">
         <v>90</v>
       </c>
-      <c r="O30" s="305"/>
-      <c r="P30" s="305"/>
-      <c r="Q30" s="305"/>
-      <c r="R30" s="305"/>
+      <c r="O30" s="294"/>
+      <c r="P30" s="294"/>
+      <c r="Q30" s="294"/>
+      <c r="R30" s="294"/>
     </row>
     <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="301" t="s">
+      <c r="B31" s="293" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="301"/>
-      <c r="D31" s="301"/>
-      <c r="E31" s="301"/>
-      <c r="F31" s="302">
+      <c r="C31" s="293"/>
+      <c r="D31" s="293"/>
+      <c r="E31" s="293"/>
+      <c r="F31" s="299">
         <v>47</v>
       </c>
-      <c r="G31" s="303"/>
-      <c r="H31" s="303"/>
+      <c r="G31" s="300"/>
+      <c r="H31" s="300"/>
       <c r="I31" s="217"/>
       <c r="J31" s="217"/>
       <c r="K31" s="217"/>
-      <c r="L31" s="301" t="s">
+      <c r="L31" s="293" t="s">
         <v>92</v>
       </c>
-      <c r="M31" s="301"/>
-      <c r="N31" s="305" t="s">
+      <c r="M31" s="293"/>
+      <c r="N31" s="294" t="s">
         <v>93</v>
       </c>
-      <c r="O31" s="305"/>
-      <c r="P31" s="305"/>
-      <c r="Q31" s="305"/>
-      <c r="R31" s="305"/>
+      <c r="O31" s="294"/>
+      <c r="P31" s="294"/>
+      <c r="Q31" s="294"/>
+      <c r="R31" s="294"/>
     </row>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="301" t="s">
+      <c r="B32" s="293" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="301"/>
-      <c r="D32" s="301"/>
-      <c r="E32" s="301"/>
-      <c r="F32" s="302">
+      <c r="C32" s="293"/>
+      <c r="D32" s="293"/>
+      <c r="E32" s="293"/>
+      <c r="F32" s="299">
         <v>10</v>
       </c>
-      <c r="G32" s="303"/>
-      <c r="H32" s="303"/>
+      <c r="G32" s="300"/>
+      <c r="H32" s="300"/>
       <c r="I32" s="217"/>
       <c r="J32" s="217"/>
       <c r="K32" s="217"/>
@@ -25470,6 +25474,36 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A7:A21"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="K7:K21"/>
+    <mergeCell ref="L7:S7"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="Q1:S4"/>
+    <mergeCell ref="L6:S6"/>
+    <mergeCell ref="F1:O4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="L25:R25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="N29:R29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:R30"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
     <mergeCell ref="A35:D38"/>
     <mergeCell ref="F35:I38"/>
     <mergeCell ref="K35:N38"/>
@@ -25480,36 +25514,6 @@
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="N29:R29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:R30"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="L25:R25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="A7:A21"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="K7:K21"/>
-    <mergeCell ref="L7:S7"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="Q1:S4"/>
-    <mergeCell ref="L6:S6"/>
-    <mergeCell ref="F1:O4"/>
-    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="3.937007874015748E-2" top="0.15748031496062992" bottom="0.15748031496062992" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -29690,215 +29694,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="334"/>
-      <c r="B1" s="334"/>
-      <c r="C1" s="334"/>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
+      <c r="A1" s="339"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
       <c r="F1" s="311" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
-      <c r="P1" s="336"/>
-      <c r="Q1" s="336"/>
-      <c r="R1" s="336"/>
-      <c r="S1" s="336"/>
-      <c r="T1" s="336"/>
-      <c r="U1" s="336"/>
-      <c r="V1" s="336"/>
-      <c r="W1" s="334"/>
-      <c r="X1" s="334"/>
-      <c r="Y1" s="334"/>
-      <c r="Z1" s="334"/>
-      <c r="AA1" s="334"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="341"/>
+      <c r="I1" s="341"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="341"/>
+      <c r="L1" s="341"/>
+      <c r="M1" s="341"/>
+      <c r="N1" s="341"/>
+      <c r="O1" s="341"/>
+      <c r="P1" s="341"/>
+      <c r="Q1" s="341"/>
+      <c r="R1" s="341"/>
+      <c r="S1" s="341"/>
+      <c r="T1" s="341"/>
+      <c r="U1" s="341"/>
+      <c r="V1" s="341"/>
+      <c r="W1" s="339"/>
+      <c r="X1" s="339"/>
+      <c r="Y1" s="339"/>
+      <c r="Z1" s="339"/>
+      <c r="AA1" s="339"/>
     </row>
     <row r="2" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="334"/>
-      <c r="B2" s="334"/>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336"/>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336"/>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
-      <c r="T2" s="336"/>
-      <c r="U2" s="336"/>
-      <c r="V2" s="336"/>
-      <c r="W2" s="334"/>
-      <c r="X2" s="334"/>
-      <c r="Y2" s="334"/>
-      <c r="Z2" s="334"/>
-      <c r="AA2" s="334"/>
+      <c r="A2" s="339"/>
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
+      <c r="K2" s="341"/>
+      <c r="L2" s="341"/>
+      <c r="M2" s="341"/>
+      <c r="N2" s="341"/>
+      <c r="O2" s="341"/>
+      <c r="P2" s="341"/>
+      <c r="Q2" s="341"/>
+      <c r="R2" s="341"/>
+      <c r="S2" s="341"/>
+      <c r="T2" s="341"/>
+      <c r="U2" s="341"/>
+      <c r="V2" s="341"/>
+      <c r="W2" s="339"/>
+      <c r="X2" s="339"/>
+      <c r="Y2" s="339"/>
+      <c r="Z2" s="339"/>
+      <c r="AA2" s="339"/>
     </row>
     <row r="3" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="334"/>
-      <c r="B3" s="334"/>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336"/>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336"/>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
-      <c r="T3" s="336"/>
-      <c r="U3" s="336"/>
-      <c r="V3" s="336"/>
-      <c r="W3" s="334"/>
-      <c r="X3" s="334"/>
-      <c r="Y3" s="334"/>
-      <c r="Z3" s="334"/>
-      <c r="AA3" s="334"/>
+      <c r="A3" s="339"/>
+      <c r="B3" s="339"/>
+      <c r="C3" s="339"/>
+      <c r="D3" s="339"/>
+      <c r="E3" s="339"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
+      <c r="K3" s="341"/>
+      <c r="L3" s="341"/>
+      <c r="M3" s="341"/>
+      <c r="N3" s="341"/>
+      <c r="O3" s="341"/>
+      <c r="P3" s="341"/>
+      <c r="Q3" s="341"/>
+      <c r="R3" s="341"/>
+      <c r="S3" s="341"/>
+      <c r="T3" s="341"/>
+      <c r="U3" s="341"/>
+      <c r="V3" s="341"/>
+      <c r="W3" s="339"/>
+      <c r="X3" s="339"/>
+      <c r="Y3" s="339"/>
+      <c r="Z3" s="339"/>
+      <c r="AA3" s="339"/>
     </row>
     <row r="4" spans="1:47" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="335"/>
-      <c r="B4" s="335"/>
-      <c r="C4" s="335"/>
-      <c r="D4" s="335"/>
-      <c r="E4" s="335"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="337"/>
-      <c r="L4" s="337"/>
-      <c r="M4" s="337"/>
-      <c r="N4" s="337"/>
-      <c r="O4" s="337"/>
-      <c r="P4" s="337"/>
-      <c r="Q4" s="337"/>
-      <c r="R4" s="337"/>
-      <c r="S4" s="337"/>
-      <c r="T4" s="337"/>
-      <c r="U4" s="337"/>
-      <c r="V4" s="337"/>
-      <c r="W4" s="335"/>
-      <c r="X4" s="335"/>
-      <c r="Y4" s="335"/>
-      <c r="Z4" s="335"/>
-      <c r="AA4" s="335"/>
+      <c r="A4" s="340"/>
+      <c r="B4" s="340"/>
+      <c r="C4" s="340"/>
+      <c r="D4" s="340"/>
+      <c r="E4" s="340"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="342"/>
+      <c r="N4" s="342"/>
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="342"/>
+      <c r="U4" s="342"/>
+      <c r="V4" s="342"/>
+      <c r="W4" s="340"/>
+      <c r="X4" s="340"/>
+      <c r="Y4" s="340"/>
+      <c r="Z4" s="340"/>
+      <c r="AA4" s="340"/>
     </row>
     <row r="5" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="338" t="s">
+      <c r="A5" s="343" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="338"/>
-      <c r="C5" s="338"/>
-      <c r="D5" s="338"/>
-      <c r="E5" s="338"/>
-      <c r="F5" s="338"/>
-      <c r="G5" s="338"/>
-      <c r="H5" s="338"/>
-      <c r="I5" s="338"/>
-      <c r="J5" s="338"/>
-      <c r="K5" s="338"/>
-      <c r="L5" s="338"/>
-      <c r="M5" s="338"/>
-      <c r="N5" s="338"/>
-      <c r="O5" s="338"/>
-      <c r="P5" s="338"/>
-      <c r="Q5" s="338"/>
-      <c r="R5" s="338"/>
-      <c r="S5" s="338"/>
-      <c r="T5" s="338"/>
-      <c r="U5" s="338"/>
-      <c r="V5" s="338"/>
-      <c r="W5" s="338"/>
-      <c r="X5" s="340" t="s">
+      <c r="B5" s="343"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
+      <c r="E5" s="343"/>
+      <c r="F5" s="343"/>
+      <c r="G5" s="343"/>
+      <c r="H5" s="343"/>
+      <c r="I5" s="343"/>
+      <c r="J5" s="343"/>
+      <c r="K5" s="343"/>
+      <c r="L5" s="343"/>
+      <c r="M5" s="343"/>
+      <c r="N5" s="343"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="343"/>
+      <c r="Q5" s="343"/>
+      <c r="R5" s="343"/>
+      <c r="S5" s="343"/>
+      <c r="T5" s="343"/>
+      <c r="U5" s="343"/>
+      <c r="V5" s="343"/>
+      <c r="W5" s="343"/>
+      <c r="X5" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="340"/>
-      <c r="Z5" s="340"/>
-      <c r="AA5" s="340"/>
+      <c r="Y5" s="345"/>
+      <c r="Z5" s="345"/>
+      <c r="AA5" s="345"/>
     </row>
     <row r="6" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="339"/>
-      <c r="B6" s="339"/>
-      <c r="C6" s="339"/>
-      <c r="D6" s="339"/>
-      <c r="E6" s="339"/>
-      <c r="F6" s="339"/>
-      <c r="G6" s="339"/>
-      <c r="H6" s="339"/>
-      <c r="I6" s="339"/>
-      <c r="J6" s="339"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="339"/>
-      <c r="M6" s="339"/>
-      <c r="N6" s="339"/>
-      <c r="O6" s="339"/>
-      <c r="P6" s="339"/>
-      <c r="Q6" s="339"/>
-      <c r="R6" s="339"/>
-      <c r="S6" s="339"/>
-      <c r="T6" s="339"/>
-      <c r="U6" s="339"/>
-      <c r="V6" s="339"/>
-      <c r="W6" s="339"/>
-      <c r="X6" s="341"/>
-      <c r="Y6" s="341"/>
-      <c r="Z6" s="341"/>
-      <c r="AA6" s="341"/>
+      <c r="A6" s="344"/>
+      <c r="B6" s="344"/>
+      <c r="C6" s="344"/>
+      <c r="D6" s="344"/>
+      <c r="E6" s="344"/>
+      <c r="F6" s="344"/>
+      <c r="G6" s="344"/>
+      <c r="H6" s="344"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
+      <c r="K6" s="344"/>
+      <c r="L6" s="344"/>
+      <c r="M6" s="344"/>
+      <c r="N6" s="344"/>
+      <c r="O6" s="344"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="344"/>
+      <c r="R6" s="344"/>
+      <c r="S6" s="344"/>
+      <c r="T6" s="344"/>
+      <c r="U6" s="344"/>
+      <c r="V6" s="344"/>
+      <c r="W6" s="344"/>
+      <c r="X6" s="346"/>
+      <c r="Y6" s="346"/>
+      <c r="Z6" s="346"/>
+      <c r="AA6" s="346"/>
     </row>
     <row r="7" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="333" t="s">
+      <c r="A7" s="338" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="333"/>
-      <c r="C7" s="333"/>
-      <c r="D7" s="333"/>
-      <c r="E7" s="333"/>
-      <c r="F7" s="333"/>
-      <c r="G7" s="333"/>
-      <c r="H7" s="333"/>
-      <c r="I7" s="333"/>
-      <c r="J7" s="333"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="333"/>
-      <c r="M7" s="333"/>
-      <c r="N7" s="333"/>
-      <c r="O7" s="333"/>
-      <c r="P7" s="333"/>
-      <c r="Q7" s="333"/>
-      <c r="R7" s="333"/>
-      <c r="S7" s="333"/>
-      <c r="T7" s="333"/>
-      <c r="U7" s="333"/>
-      <c r="V7" s="333"/>
-      <c r="W7" s="333"/>
-      <c r="X7" s="333"/>
-      <c r="Y7" s="333"/>
-      <c r="Z7" s="333"/>
-      <c r="AA7" s="333"/>
+      <c r="B7" s="338"/>
+      <c r="C7" s="338"/>
+      <c r="D7" s="338"/>
+      <c r="E7" s="338"/>
+      <c r="F7" s="338"/>
+      <c r="G7" s="338"/>
+      <c r="H7" s="338"/>
+      <c r="I7" s="338"/>
+      <c r="J7" s="338"/>
+      <c r="K7" s="338"/>
+      <c r="L7" s="338"/>
+      <c r="M7" s="338"/>
+      <c r="N7" s="338"/>
+      <c r="O7" s="338"/>
+      <c r="P7" s="338"/>
+      <c r="Q7" s="338"/>
+      <c r="R7" s="338"/>
+      <c r="S7" s="338"/>
+      <c r="T7" s="338"/>
+      <c r="U7" s="338"/>
+      <c r="V7" s="338"/>
+      <c r="W7" s="338"/>
+      <c r="X7" s="338"/>
+      <c r="Y7" s="338"/>
+      <c r="Z7" s="338"/>
+      <c r="AA7" s="338"/>
     </row>
     <row r="8" spans="1:47" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98"/>
@@ -29993,24 +29997,24 @@
       <c r="C11" s="97"/>
       <c r="D11" s="97"/>
       <c r="E11" s="97"/>
-      <c r="F11" s="345" t="s">
+      <c r="F11" s="336" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="346" t="s">
+      <c r="G11" s="337" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="346"/>
-      <c r="I11" s="346"/>
-      <c r="J11" s="346"/>
-      <c r="K11" s="346"/>
-      <c r="L11" s="346"/>
-      <c r="M11" s="346"/>
-      <c r="N11" s="346"/>
-      <c r="O11" s="346"/>
-      <c r="P11" s="346"/>
-      <c r="Q11" s="346"/>
-      <c r="R11" s="346"/>
-      <c r="S11" s="346"/>
+      <c r="H11" s="337"/>
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+      <c r="K11" s="337"/>
+      <c r="L11" s="337"/>
+      <c r="M11" s="337"/>
+      <c r="N11" s="337"/>
+      <c r="O11" s="337"/>
+      <c r="P11" s="337"/>
+      <c r="Q11" s="337"/>
+      <c r="R11" s="337"/>
+      <c r="S11" s="337"/>
       <c r="T11" s="92"/>
       <c r="U11" s="92"/>
       <c r="V11" s="92"/>
@@ -30026,7 +30030,7 @@
       <c r="C12" s="97"/>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
-      <c r="F12" s="345"/>
+      <c r="F12" s="336"/>
       <c r="G12" s="226">
         <v>100</v>
       </c>
@@ -30074,7 +30078,7 @@
       <c r="Y12" s="97"/>
       <c r="Z12" s="97"/>
       <c r="AA12" s="97"/>
-      <c r="AE12" s="344"/>
+      <c r="AE12" s="335"/>
       <c r="AF12" s="92"/>
       <c r="AG12" s="92"/>
       <c r="AH12" s="92"/>
@@ -30148,7 +30152,7 @@
       <c r="Y13" s="97"/>
       <c r="Z13" s="97"/>
       <c r="AA13" s="97"/>
-      <c r="AE13" s="344"/>
+      <c r="AE13" s="335"/>
       <c r="AF13" s="93"/>
       <c r="AG13" s="93"/>
       <c r="AH13" s="93"/>
@@ -31236,13 +31240,13 @@
       <c r="C40" s="280"/>
       <c r="D40" s="280"/>
       <c r="E40" s="280"/>
-      <c r="H40" s="342" t="s">
+      <c r="H40" s="333" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="342"/>
-      <c r="J40" s="342"/>
-      <c r="K40" s="342"/>
-      <c r="L40" s="342"/>
+      <c r="I40" s="333"/>
+      <c r="J40" s="333"/>
+      <c r="K40" s="333"/>
+      <c r="L40" s="333"/>
       <c r="P40" s="280" t="s">
         <v>177</v>
       </c>
@@ -31264,11 +31268,11 @@
       <c r="C41" s="268"/>
       <c r="D41" s="268"/>
       <c r="E41" s="268"/>
-      <c r="H41" s="343"/>
-      <c r="I41" s="343"/>
-      <c r="J41" s="343"/>
-      <c r="K41" s="343"/>
-      <c r="L41" s="343"/>
+      <c r="H41" s="334"/>
+      <c r="I41" s="334"/>
+      <c r="J41" s="334"/>
+      <c r="K41" s="334"/>
+      <c r="L41" s="334"/>
       <c r="P41" s="268"/>
       <c r="Q41" s="268"/>
       <c r="R41" s="268"/>
@@ -31286,11 +31290,11 @@
       <c r="C42" s="268"/>
       <c r="D42" s="268"/>
       <c r="E42" s="268"/>
-      <c r="H42" s="343"/>
-      <c r="I42" s="343"/>
-      <c r="J42" s="343"/>
-      <c r="K42" s="343"/>
-      <c r="L42" s="343"/>
+      <c r="H42" s="334"/>
+      <c r="I42" s="334"/>
+      <c r="J42" s="334"/>
+      <c r="K42" s="334"/>
+      <c r="L42" s="334"/>
       <c r="P42" s="268"/>
       <c r="Q42" s="268"/>
       <c r="R42" s="268"/>
@@ -31308,11 +31312,11 @@
       <c r="C43" s="268"/>
       <c r="D43" s="268"/>
       <c r="E43" s="268"/>
-      <c r="H43" s="343"/>
-      <c r="I43" s="343"/>
-      <c r="J43" s="343"/>
-      <c r="K43" s="343"/>
-      <c r="L43" s="343"/>
+      <c r="H43" s="334"/>
+      <c r="I43" s="334"/>
+      <c r="J43" s="334"/>
+      <c r="K43" s="334"/>
+      <c r="L43" s="334"/>
       <c r="P43" s="268"/>
       <c r="Q43" s="268"/>
       <c r="R43" s="268"/>
@@ -31326,6 +31330,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A7:AA7"/>
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="F1:V4"/>
+    <mergeCell ref="W1:AA4"/>
+    <mergeCell ref="A5:W6"/>
+    <mergeCell ref="X5:AA6"/>
     <mergeCell ref="A40:E43"/>
     <mergeCell ref="H40:L43"/>
     <mergeCell ref="P40:T43"/>
@@ -31333,12 +31343,6 @@
     <mergeCell ref="AE12:AE13"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:S11"/>
-    <mergeCell ref="A7:AA7"/>
-    <mergeCell ref="A1:E4"/>
-    <mergeCell ref="F1:V4"/>
-    <mergeCell ref="W1:AA4"/>
-    <mergeCell ref="A5:W6"/>
-    <mergeCell ref="X5:AA6"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -33393,8 +33397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8082F7-C7B4-4F21-8B67-9FEB3EE2E7B5}">
   <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33459,7 +33463,7 @@
       <c r="R1" s="240">
         <v>479</v>
       </c>
-      <c r="S1" s="242">
+      <c r="S1" s="382">
         <v>500</v>
       </c>
       <c r="T1" s="240">
@@ -33489,7 +33493,7 @@
       <c r="AB1" s="240">
         <v>685</v>
       </c>
-      <c r="AC1" s="242">
+      <c r="AC1" s="382">
         <v>706</v>
       </c>
       <c r="AD1" s="244">
@@ -39355,7 +39359,7 @@
       <c r="V22" s="257"/>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="344"/>
+      <c r="A48" s="335"/>
       <c r="B48" s="349"/>
       <c r="C48" s="349"/>
       <c r="D48" s="349"/>
@@ -39379,7 +39383,7 @@
       <c r="V48" s="349"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="344"/>
+      <c r="A49" s="335"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B54" s="93"/>
@@ -41200,215 +41204,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="334"/>
-      <c r="B1" s="334"/>
-      <c r="C1" s="334"/>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
+      <c r="A1" s="339"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
       <c r="F1" s="311" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
-      <c r="P1" s="336"/>
-      <c r="Q1" s="336"/>
-      <c r="R1" s="336"/>
-      <c r="S1" s="336"/>
-      <c r="T1" s="336"/>
-      <c r="U1" s="336"/>
-      <c r="V1" s="336"/>
-      <c r="W1" s="334"/>
-      <c r="X1" s="334"/>
-      <c r="Y1" s="334"/>
-      <c r="Z1" s="334"/>
-      <c r="AA1" s="334"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="341"/>
+      <c r="I1" s="341"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="341"/>
+      <c r="L1" s="341"/>
+      <c r="M1" s="341"/>
+      <c r="N1" s="341"/>
+      <c r="O1" s="341"/>
+      <c r="P1" s="341"/>
+      <c r="Q1" s="341"/>
+      <c r="R1" s="341"/>
+      <c r="S1" s="341"/>
+      <c r="T1" s="341"/>
+      <c r="U1" s="341"/>
+      <c r="V1" s="341"/>
+      <c r="W1" s="339"/>
+      <c r="X1" s="339"/>
+      <c r="Y1" s="339"/>
+      <c r="Z1" s="339"/>
+      <c r="AA1" s="339"/>
     </row>
     <row r="2" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="334"/>
-      <c r="B2" s="334"/>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336"/>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336"/>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
-      <c r="T2" s="336"/>
-      <c r="U2" s="336"/>
-      <c r="V2" s="336"/>
-      <c r="W2" s="334"/>
-      <c r="X2" s="334"/>
-      <c r="Y2" s="334"/>
-      <c r="Z2" s="334"/>
-      <c r="AA2" s="334"/>
+      <c r="A2" s="339"/>
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
+      <c r="K2" s="341"/>
+      <c r="L2" s="341"/>
+      <c r="M2" s="341"/>
+      <c r="N2" s="341"/>
+      <c r="O2" s="341"/>
+      <c r="P2" s="341"/>
+      <c r="Q2" s="341"/>
+      <c r="R2" s="341"/>
+      <c r="S2" s="341"/>
+      <c r="T2" s="341"/>
+      <c r="U2" s="341"/>
+      <c r="V2" s="341"/>
+      <c r="W2" s="339"/>
+      <c r="X2" s="339"/>
+      <c r="Y2" s="339"/>
+      <c r="Z2" s="339"/>
+      <c r="AA2" s="339"/>
     </row>
     <row r="3" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="334"/>
-      <c r="B3" s="334"/>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336"/>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336"/>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
-      <c r="T3" s="336"/>
-      <c r="U3" s="336"/>
-      <c r="V3" s="336"/>
-      <c r="W3" s="334"/>
-      <c r="X3" s="334"/>
-      <c r="Y3" s="334"/>
-      <c r="Z3" s="334"/>
-      <c r="AA3" s="334"/>
+      <c r="A3" s="339"/>
+      <c r="B3" s="339"/>
+      <c r="C3" s="339"/>
+      <c r="D3" s="339"/>
+      <c r="E3" s="339"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
+      <c r="K3" s="341"/>
+      <c r="L3" s="341"/>
+      <c r="M3" s="341"/>
+      <c r="N3" s="341"/>
+      <c r="O3" s="341"/>
+      <c r="P3" s="341"/>
+      <c r="Q3" s="341"/>
+      <c r="R3" s="341"/>
+      <c r="S3" s="341"/>
+      <c r="T3" s="341"/>
+      <c r="U3" s="341"/>
+      <c r="V3" s="341"/>
+      <c r="W3" s="339"/>
+      <c r="X3" s="339"/>
+      <c r="Y3" s="339"/>
+      <c r="Z3" s="339"/>
+      <c r="AA3" s="339"/>
     </row>
     <row r="4" spans="1:47" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="335"/>
-      <c r="B4" s="335"/>
-      <c r="C4" s="335"/>
-      <c r="D4" s="335"/>
-      <c r="E4" s="335"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="337"/>
-      <c r="L4" s="337"/>
-      <c r="M4" s="337"/>
-      <c r="N4" s="337"/>
-      <c r="O4" s="337"/>
-      <c r="P4" s="337"/>
-      <c r="Q4" s="337"/>
-      <c r="R4" s="337"/>
-      <c r="S4" s="337"/>
-      <c r="T4" s="337"/>
-      <c r="U4" s="337"/>
-      <c r="V4" s="337"/>
-      <c r="W4" s="335"/>
-      <c r="X4" s="335"/>
-      <c r="Y4" s="335"/>
-      <c r="Z4" s="335"/>
-      <c r="AA4" s="335"/>
+      <c r="A4" s="340"/>
+      <c r="B4" s="340"/>
+      <c r="C4" s="340"/>
+      <c r="D4" s="340"/>
+      <c r="E4" s="340"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="342"/>
+      <c r="N4" s="342"/>
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="342"/>
+      <c r="U4" s="342"/>
+      <c r="V4" s="342"/>
+      <c r="W4" s="340"/>
+      <c r="X4" s="340"/>
+      <c r="Y4" s="340"/>
+      <c r="Z4" s="340"/>
+      <c r="AA4" s="340"/>
     </row>
     <row r="5" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="338" t="s">
+      <c r="A5" s="343" t="s">
         <v>207</v>
       </c>
-      <c r="B5" s="338"/>
-      <c r="C5" s="338"/>
-      <c r="D5" s="338"/>
-      <c r="E5" s="338"/>
-      <c r="F5" s="338"/>
-      <c r="G5" s="338"/>
-      <c r="H5" s="338"/>
-      <c r="I5" s="338"/>
-      <c r="J5" s="338"/>
-      <c r="K5" s="338"/>
-      <c r="L5" s="338"/>
-      <c r="M5" s="338"/>
-      <c r="N5" s="338"/>
-      <c r="O5" s="338"/>
-      <c r="P5" s="338"/>
-      <c r="Q5" s="338"/>
-      <c r="R5" s="338"/>
-      <c r="S5" s="338"/>
-      <c r="T5" s="338"/>
-      <c r="U5" s="338"/>
-      <c r="V5" s="338"/>
-      <c r="W5" s="338"/>
-      <c r="X5" s="340" t="s">
+      <c r="B5" s="343"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
+      <c r="E5" s="343"/>
+      <c r="F5" s="343"/>
+      <c r="G5" s="343"/>
+      <c r="H5" s="343"/>
+      <c r="I5" s="343"/>
+      <c r="J5" s="343"/>
+      <c r="K5" s="343"/>
+      <c r="L5" s="343"/>
+      <c r="M5" s="343"/>
+      <c r="N5" s="343"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="343"/>
+      <c r="Q5" s="343"/>
+      <c r="R5" s="343"/>
+      <c r="S5" s="343"/>
+      <c r="T5" s="343"/>
+      <c r="U5" s="343"/>
+      <c r="V5" s="343"/>
+      <c r="W5" s="343"/>
+      <c r="X5" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="340"/>
-      <c r="Z5" s="340"/>
-      <c r="AA5" s="340"/>
+      <c r="Y5" s="345"/>
+      <c r="Z5" s="345"/>
+      <c r="AA5" s="345"/>
     </row>
     <row r="6" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="339"/>
-      <c r="B6" s="339"/>
-      <c r="C6" s="339"/>
-      <c r="D6" s="339"/>
-      <c r="E6" s="339"/>
-      <c r="F6" s="339"/>
-      <c r="G6" s="339"/>
-      <c r="H6" s="339"/>
-      <c r="I6" s="339"/>
-      <c r="J6" s="339"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="339"/>
-      <c r="M6" s="339"/>
-      <c r="N6" s="339"/>
-      <c r="O6" s="339"/>
-      <c r="P6" s="339"/>
-      <c r="Q6" s="339"/>
-      <c r="R6" s="339"/>
-      <c r="S6" s="339"/>
-      <c r="T6" s="339"/>
-      <c r="U6" s="339"/>
-      <c r="V6" s="339"/>
-      <c r="W6" s="339"/>
-      <c r="X6" s="341"/>
-      <c r="Y6" s="341"/>
-      <c r="Z6" s="341"/>
-      <c r="AA6" s="341"/>
+      <c r="A6" s="344"/>
+      <c r="B6" s="344"/>
+      <c r="C6" s="344"/>
+      <c r="D6" s="344"/>
+      <c r="E6" s="344"/>
+      <c r="F6" s="344"/>
+      <c r="G6" s="344"/>
+      <c r="H6" s="344"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
+      <c r="K6" s="344"/>
+      <c r="L6" s="344"/>
+      <c r="M6" s="344"/>
+      <c r="N6" s="344"/>
+      <c r="O6" s="344"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="344"/>
+      <c r="R6" s="344"/>
+      <c r="S6" s="344"/>
+      <c r="T6" s="344"/>
+      <c r="U6" s="344"/>
+      <c r="V6" s="344"/>
+      <c r="W6" s="344"/>
+      <c r="X6" s="346"/>
+      <c r="Y6" s="346"/>
+      <c r="Z6" s="346"/>
+      <c r="AA6" s="346"/>
     </row>
     <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="333" t="s">
+      <c r="A7" s="338" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="333"/>
-      <c r="C7" s="333"/>
-      <c r="D7" s="333"/>
-      <c r="E7" s="333"/>
-      <c r="F7" s="333"/>
-      <c r="G7" s="333"/>
-      <c r="H7" s="333"/>
-      <c r="I7" s="333"/>
-      <c r="J7" s="333"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="333"/>
-      <c r="M7" s="333"/>
-      <c r="N7" s="333"/>
-      <c r="O7" s="333"/>
-      <c r="P7" s="333"/>
-      <c r="Q7" s="333"/>
-      <c r="R7" s="333"/>
-      <c r="S7" s="333"/>
-      <c r="T7" s="333"/>
-      <c r="U7" s="333"/>
-      <c r="V7" s="333"/>
-      <c r="W7" s="333"/>
-      <c r="X7" s="333"/>
-      <c r="Y7" s="333"/>
-      <c r="Z7" s="333"/>
-      <c r="AA7" s="333"/>
+      <c r="B7" s="338"/>
+      <c r="C7" s="338"/>
+      <c r="D7" s="338"/>
+      <c r="E7" s="338"/>
+      <c r="F7" s="338"/>
+      <c r="G7" s="338"/>
+      <c r="H7" s="338"/>
+      <c r="I7" s="338"/>
+      <c r="J7" s="338"/>
+      <c r="K7" s="338"/>
+      <c r="L7" s="338"/>
+      <c r="M7" s="338"/>
+      <c r="N7" s="338"/>
+      <c r="O7" s="338"/>
+      <c r="P7" s="338"/>
+      <c r="Q7" s="338"/>
+      <c r="R7" s="338"/>
+      <c r="S7" s="338"/>
+      <c r="T7" s="338"/>
+      <c r="U7" s="338"/>
+      <c r="V7" s="338"/>
+      <c r="W7" s="338"/>
+      <c r="X7" s="338"/>
+      <c r="Y7" s="338"/>
+      <c r="Z7" s="338"/>
+      <c r="AA7" s="338"/>
     </row>
     <row r="8" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98"/>
@@ -41520,24 +41524,24 @@
       <c r="C11" s="97"/>
       <c r="D11" s="97"/>
       <c r="E11" s="97"/>
-      <c r="F11" s="345" t="s">
+      <c r="F11" s="336" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="346" t="s">
+      <c r="G11" s="337" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="346"/>
-      <c r="I11" s="346"/>
-      <c r="J11" s="346"/>
-      <c r="K11" s="346"/>
-      <c r="L11" s="346"/>
-      <c r="M11" s="346"/>
-      <c r="N11" s="346"/>
-      <c r="O11" s="346"/>
-      <c r="P11" s="346"/>
-      <c r="Q11" s="346"/>
-      <c r="R11" s="346"/>
-      <c r="S11" s="346"/>
+      <c r="H11" s="337"/>
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+      <c r="K11" s="337"/>
+      <c r="L11" s="337"/>
+      <c r="M11" s="337"/>
+      <c r="N11" s="337"/>
+      <c r="O11" s="337"/>
+      <c r="P11" s="337"/>
+      <c r="Q11" s="337"/>
+      <c r="R11" s="337"/>
+      <c r="S11" s="337"/>
       <c r="T11" s="92"/>
       <c r="U11" s="92"/>
       <c r="V11" s="92"/>
@@ -41570,7 +41574,7 @@
       <c r="C12" s="97"/>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
-      <c r="F12" s="345"/>
+      <c r="F12" s="336"/>
       <c r="G12" s="226">
         <v>100</v>
       </c>
@@ -42871,13 +42875,13 @@
       <c r="C41" s="280"/>
       <c r="D41" s="280"/>
       <c r="E41" s="280"/>
-      <c r="H41" s="342" t="s">
+      <c r="H41" s="333" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="342"/>
-      <c r="J41" s="342"/>
-      <c r="K41" s="342"/>
-      <c r="L41" s="342"/>
+      <c r="I41" s="333"/>
+      <c r="J41" s="333"/>
+      <c r="K41" s="333"/>
+      <c r="L41" s="333"/>
       <c r="P41" s="280" t="s">
         <v>177</v>
       </c>
@@ -42899,11 +42903,11 @@
       <c r="C42" s="268"/>
       <c r="D42" s="268"/>
       <c r="E42" s="268"/>
-      <c r="H42" s="343"/>
-      <c r="I42" s="343"/>
-      <c r="J42" s="343"/>
-      <c r="K42" s="343"/>
-      <c r="L42" s="343"/>
+      <c r="H42" s="334"/>
+      <c r="I42" s="334"/>
+      <c r="J42" s="334"/>
+      <c r="K42" s="334"/>
+      <c r="L42" s="334"/>
       <c r="P42" s="268"/>
       <c r="Q42" s="268"/>
       <c r="R42" s="268"/>
@@ -42921,11 +42925,11 @@
       <c r="C43" s="268"/>
       <c r="D43" s="268"/>
       <c r="E43" s="268"/>
-      <c r="H43" s="343"/>
-      <c r="I43" s="343"/>
-      <c r="J43" s="343"/>
-      <c r="K43" s="343"/>
-      <c r="L43" s="343"/>
+      <c r="H43" s="334"/>
+      <c r="I43" s="334"/>
+      <c r="J43" s="334"/>
+      <c r="K43" s="334"/>
+      <c r="L43" s="334"/>
       <c r="P43" s="268"/>
       <c r="Q43" s="268"/>
       <c r="R43" s="268"/>
@@ -42943,11 +42947,11 @@
       <c r="C44" s="268"/>
       <c r="D44" s="268"/>
       <c r="E44" s="268"/>
-      <c r="H44" s="343"/>
-      <c r="I44" s="343"/>
-      <c r="J44" s="343"/>
-      <c r="K44" s="343"/>
-      <c r="L44" s="343"/>
+      <c r="H44" s="334"/>
+      <c r="I44" s="334"/>
+      <c r="J44" s="334"/>
+      <c r="K44" s="334"/>
+      <c r="L44" s="334"/>
       <c r="P44" s="268"/>
       <c r="Q44" s="268"/>
       <c r="R44" s="268"/>
@@ -42961,18 +42965,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:AA7"/>
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="F1:V4"/>
+    <mergeCell ref="W1:AA4"/>
+    <mergeCell ref="A5:W6"/>
+    <mergeCell ref="X5:AA6"/>
     <mergeCell ref="A41:E44"/>
     <mergeCell ref="H41:L44"/>
     <mergeCell ref="P41:T44"/>
     <mergeCell ref="W41:AA44"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:S11"/>
-    <mergeCell ref="A7:AA7"/>
-    <mergeCell ref="A1:E4"/>
-    <mergeCell ref="F1:V4"/>
-    <mergeCell ref="W1:AA4"/>
-    <mergeCell ref="A5:W6"/>
-    <mergeCell ref="X5:AA6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="3.937007874015748E-2" top="0.15748031496062992" bottom="0.15748031496062992" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
@@ -43000,215 +43004,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="334"/>
-      <c r="B1" s="334"/>
-      <c r="C1" s="334"/>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
+      <c r="A1" s="339"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
       <c r="F1" s="311" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
-      <c r="P1" s="336"/>
-      <c r="Q1" s="336"/>
-      <c r="R1" s="336"/>
-      <c r="S1" s="336"/>
-      <c r="T1" s="336"/>
-      <c r="U1" s="336"/>
-      <c r="V1" s="336"/>
-      <c r="W1" s="334"/>
-      <c r="X1" s="334"/>
-      <c r="Y1" s="334"/>
-      <c r="Z1" s="334"/>
-      <c r="AA1" s="334"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="341"/>
+      <c r="I1" s="341"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="341"/>
+      <c r="L1" s="341"/>
+      <c r="M1" s="341"/>
+      <c r="N1" s="341"/>
+      <c r="O1" s="341"/>
+      <c r="P1" s="341"/>
+      <c r="Q1" s="341"/>
+      <c r="R1" s="341"/>
+      <c r="S1" s="341"/>
+      <c r="T1" s="341"/>
+      <c r="U1" s="341"/>
+      <c r="V1" s="341"/>
+      <c r="W1" s="339"/>
+      <c r="X1" s="339"/>
+      <c r="Y1" s="339"/>
+      <c r="Z1" s="339"/>
+      <c r="AA1" s="339"/>
     </row>
     <row r="2" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="334"/>
-      <c r="B2" s="334"/>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336"/>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336"/>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
-      <c r="T2" s="336"/>
-      <c r="U2" s="336"/>
-      <c r="V2" s="336"/>
-      <c r="W2" s="334"/>
-      <c r="X2" s="334"/>
-      <c r="Y2" s="334"/>
-      <c r="Z2" s="334"/>
-      <c r="AA2" s="334"/>
+      <c r="A2" s="339"/>
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
+      <c r="K2" s="341"/>
+      <c r="L2" s="341"/>
+      <c r="M2" s="341"/>
+      <c r="N2" s="341"/>
+      <c r="O2" s="341"/>
+      <c r="P2" s="341"/>
+      <c r="Q2" s="341"/>
+      <c r="R2" s="341"/>
+      <c r="S2" s="341"/>
+      <c r="T2" s="341"/>
+      <c r="U2" s="341"/>
+      <c r="V2" s="341"/>
+      <c r="W2" s="339"/>
+      <c r="X2" s="339"/>
+      <c r="Y2" s="339"/>
+      <c r="Z2" s="339"/>
+      <c r="AA2" s="339"/>
     </row>
     <row r="3" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="334"/>
-      <c r="B3" s="334"/>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336"/>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336"/>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
-      <c r="T3" s="336"/>
-      <c r="U3" s="336"/>
-      <c r="V3" s="336"/>
-      <c r="W3" s="334"/>
-      <c r="X3" s="334"/>
-      <c r="Y3" s="334"/>
-      <c r="Z3" s="334"/>
-      <c r="AA3" s="334"/>
+      <c r="A3" s="339"/>
+      <c r="B3" s="339"/>
+      <c r="C3" s="339"/>
+      <c r="D3" s="339"/>
+      <c r="E3" s="339"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
+      <c r="K3" s="341"/>
+      <c r="L3" s="341"/>
+      <c r="M3" s="341"/>
+      <c r="N3" s="341"/>
+      <c r="O3" s="341"/>
+      <c r="P3" s="341"/>
+      <c r="Q3" s="341"/>
+      <c r="R3" s="341"/>
+      <c r="S3" s="341"/>
+      <c r="T3" s="341"/>
+      <c r="U3" s="341"/>
+      <c r="V3" s="341"/>
+      <c r="W3" s="339"/>
+      <c r="X3" s="339"/>
+      <c r="Y3" s="339"/>
+      <c r="Z3" s="339"/>
+      <c r="AA3" s="339"/>
     </row>
     <row r="4" spans="1:47" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="335"/>
-      <c r="B4" s="335"/>
-      <c r="C4" s="335"/>
-      <c r="D4" s="335"/>
-      <c r="E4" s="335"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="337"/>
-      <c r="L4" s="337"/>
-      <c r="M4" s="337"/>
-      <c r="N4" s="337"/>
-      <c r="O4" s="337"/>
-      <c r="P4" s="337"/>
-      <c r="Q4" s="337"/>
-      <c r="R4" s="337"/>
-      <c r="S4" s="337"/>
-      <c r="T4" s="337"/>
-      <c r="U4" s="337"/>
-      <c r="V4" s="337"/>
-      <c r="W4" s="335"/>
-      <c r="X4" s="335"/>
-      <c r="Y4" s="335"/>
-      <c r="Z4" s="335"/>
-      <c r="AA4" s="335"/>
+      <c r="A4" s="340"/>
+      <c r="B4" s="340"/>
+      <c r="C4" s="340"/>
+      <c r="D4" s="340"/>
+      <c r="E4" s="340"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="342"/>
+      <c r="N4" s="342"/>
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="342"/>
+      <c r="U4" s="342"/>
+      <c r="V4" s="342"/>
+      <c r="W4" s="340"/>
+      <c r="X4" s="340"/>
+      <c r="Y4" s="340"/>
+      <c r="Z4" s="340"/>
+      <c r="AA4" s="340"/>
     </row>
     <row r="5" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="338" t="s">
+      <c r="A5" s="343" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="338"/>
-      <c r="C5" s="338"/>
-      <c r="D5" s="338"/>
-      <c r="E5" s="338"/>
-      <c r="F5" s="338"/>
-      <c r="G5" s="338"/>
-      <c r="H5" s="338"/>
-      <c r="I5" s="338"/>
-      <c r="J5" s="338"/>
-      <c r="K5" s="338"/>
-      <c r="L5" s="338"/>
-      <c r="M5" s="338"/>
-      <c r="N5" s="338"/>
-      <c r="O5" s="338"/>
-      <c r="P5" s="338"/>
-      <c r="Q5" s="338"/>
-      <c r="R5" s="338"/>
-      <c r="S5" s="338"/>
-      <c r="T5" s="338"/>
-      <c r="U5" s="338"/>
-      <c r="V5" s="338"/>
-      <c r="W5" s="338"/>
-      <c r="X5" s="340" t="s">
+      <c r="B5" s="343"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
+      <c r="E5" s="343"/>
+      <c r="F5" s="343"/>
+      <c r="G5" s="343"/>
+      <c r="H5" s="343"/>
+      <c r="I5" s="343"/>
+      <c r="J5" s="343"/>
+      <c r="K5" s="343"/>
+      <c r="L5" s="343"/>
+      <c r="M5" s="343"/>
+      <c r="N5" s="343"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="343"/>
+      <c r="Q5" s="343"/>
+      <c r="R5" s="343"/>
+      <c r="S5" s="343"/>
+      <c r="T5" s="343"/>
+      <c r="U5" s="343"/>
+      <c r="V5" s="343"/>
+      <c r="W5" s="343"/>
+      <c r="X5" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="340"/>
-      <c r="Z5" s="340"/>
-      <c r="AA5" s="340"/>
+      <c r="Y5" s="345"/>
+      <c r="Z5" s="345"/>
+      <c r="AA5" s="345"/>
     </row>
     <row r="6" spans="1:47" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="339"/>
-      <c r="B6" s="339"/>
-      <c r="C6" s="339"/>
-      <c r="D6" s="339"/>
-      <c r="E6" s="339"/>
-      <c r="F6" s="339"/>
-      <c r="G6" s="339"/>
-      <c r="H6" s="339"/>
-      <c r="I6" s="339"/>
-      <c r="J6" s="339"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="339"/>
-      <c r="M6" s="339"/>
-      <c r="N6" s="339"/>
-      <c r="O6" s="339"/>
-      <c r="P6" s="339"/>
-      <c r="Q6" s="339"/>
-      <c r="R6" s="339"/>
-      <c r="S6" s="339"/>
-      <c r="T6" s="339"/>
-      <c r="U6" s="339"/>
-      <c r="V6" s="339"/>
-      <c r="W6" s="339"/>
-      <c r="X6" s="341"/>
-      <c r="Y6" s="341"/>
-      <c r="Z6" s="341"/>
-      <c r="AA6" s="341"/>
+      <c r="A6" s="344"/>
+      <c r="B6" s="344"/>
+      <c r="C6" s="344"/>
+      <c r="D6" s="344"/>
+      <c r="E6" s="344"/>
+      <c r="F6" s="344"/>
+      <c r="G6" s="344"/>
+      <c r="H6" s="344"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
+      <c r="K6" s="344"/>
+      <c r="L6" s="344"/>
+      <c r="M6" s="344"/>
+      <c r="N6" s="344"/>
+      <c r="O6" s="344"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="344"/>
+      <c r="R6" s="344"/>
+      <c r="S6" s="344"/>
+      <c r="T6" s="344"/>
+      <c r="U6" s="344"/>
+      <c r="V6" s="344"/>
+      <c r="W6" s="344"/>
+      <c r="X6" s="346"/>
+      <c r="Y6" s="346"/>
+      <c r="Z6" s="346"/>
+      <c r="AA6" s="346"/>
     </row>
     <row r="7" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="333" t="s">
+      <c r="A7" s="338" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="333"/>
-      <c r="C7" s="333"/>
-      <c r="D7" s="333"/>
-      <c r="E7" s="333"/>
-      <c r="F7" s="333"/>
-      <c r="G7" s="333"/>
-      <c r="H7" s="333"/>
-      <c r="I7" s="333"/>
-      <c r="J7" s="333"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="333"/>
-      <c r="M7" s="333"/>
-      <c r="N7" s="333"/>
-      <c r="O7" s="333"/>
-      <c r="P7" s="333"/>
-      <c r="Q7" s="333"/>
-      <c r="R7" s="333"/>
-      <c r="S7" s="333"/>
-      <c r="T7" s="333"/>
-      <c r="U7" s="333"/>
-      <c r="V7" s="333"/>
-      <c r="W7" s="333"/>
-      <c r="X7" s="333"/>
-      <c r="Y7" s="333"/>
-      <c r="Z7" s="333"/>
-      <c r="AA7" s="333"/>
+      <c r="B7" s="338"/>
+      <c r="C7" s="338"/>
+      <c r="D7" s="338"/>
+      <c r="E7" s="338"/>
+      <c r="F7" s="338"/>
+      <c r="G7" s="338"/>
+      <c r="H7" s="338"/>
+      <c r="I7" s="338"/>
+      <c r="J7" s="338"/>
+      <c r="K7" s="338"/>
+      <c r="L7" s="338"/>
+      <c r="M7" s="338"/>
+      <c r="N7" s="338"/>
+      <c r="O7" s="338"/>
+      <c r="P7" s="338"/>
+      <c r="Q7" s="338"/>
+      <c r="R7" s="338"/>
+      <c r="S7" s="338"/>
+      <c r="T7" s="338"/>
+      <c r="U7" s="338"/>
+      <c r="V7" s="338"/>
+      <c r="W7" s="338"/>
+      <c r="X7" s="338"/>
+      <c r="Y7" s="338"/>
+      <c r="Z7" s="338"/>
+      <c r="AA7" s="338"/>
     </row>
     <row r="8" spans="1:47" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="98"/>
@@ -43303,24 +43307,24 @@
       <c r="C11" s="97"/>
       <c r="D11" s="97"/>
       <c r="E11" s="97"/>
-      <c r="F11" s="345" t="s">
+      <c r="F11" s="336" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="346" t="s">
+      <c r="G11" s="337" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="346"/>
-      <c r="I11" s="346"/>
-      <c r="J11" s="346"/>
-      <c r="K11" s="346"/>
-      <c r="L11" s="346"/>
-      <c r="M11" s="346"/>
-      <c r="N11" s="346"/>
-      <c r="O11" s="346"/>
-      <c r="P11" s="346"/>
-      <c r="Q11" s="346"/>
-      <c r="R11" s="346"/>
-      <c r="S11" s="346"/>
+      <c r="H11" s="337"/>
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+      <c r="K11" s="337"/>
+      <c r="L11" s="337"/>
+      <c r="M11" s="337"/>
+      <c r="N11" s="337"/>
+      <c r="O11" s="337"/>
+      <c r="P11" s="337"/>
+      <c r="Q11" s="337"/>
+      <c r="R11" s="337"/>
+      <c r="S11" s="337"/>
       <c r="T11" s="92"/>
       <c r="U11" s="92"/>
       <c r="V11" s="92"/>
@@ -43336,7 +43340,7 @@
       <c r="C12" s="97"/>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
-      <c r="F12" s="345"/>
+      <c r="F12" s="336"/>
       <c r="G12" s="226">
         <v>100</v>
       </c>
@@ -43384,7 +43388,7 @@
       <c r="Y12" s="97"/>
       <c r="Z12" s="97"/>
       <c r="AA12" s="97"/>
-      <c r="AE12" s="344"/>
+      <c r="AE12" s="335"/>
       <c r="AF12" s="92"/>
       <c r="AG12" s="92"/>
       <c r="AH12" s="92"/>
@@ -43458,7 +43462,7 @@
       <c r="Y13" s="97"/>
       <c r="Z13" s="97"/>
       <c r="AA13" s="97"/>
-      <c r="AE13" s="344"/>
+      <c r="AE13" s="335"/>
       <c r="AF13" s="93"/>
       <c r="AG13" s="93"/>
       <c r="AH13" s="93"/>
@@ -44546,13 +44550,13 @@
       <c r="C40" s="280"/>
       <c r="D40" s="280"/>
       <c r="E40" s="280"/>
-      <c r="H40" s="342" t="s">
+      <c r="H40" s="333" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="342"/>
-      <c r="J40" s="342"/>
-      <c r="K40" s="342"/>
-      <c r="L40" s="342"/>
+      <c r="I40" s="333"/>
+      <c r="J40" s="333"/>
+      <c r="K40" s="333"/>
+      <c r="L40" s="333"/>
       <c r="P40" s="280" t="s">
         <v>177</v>
       </c>
@@ -44574,11 +44578,11 @@
       <c r="C41" s="268"/>
       <c r="D41" s="268"/>
       <c r="E41" s="268"/>
-      <c r="H41" s="343"/>
-      <c r="I41" s="343"/>
-      <c r="J41" s="343"/>
-      <c r="K41" s="343"/>
-      <c r="L41" s="343"/>
+      <c r="H41" s="334"/>
+      <c r="I41" s="334"/>
+      <c r="J41" s="334"/>
+      <c r="K41" s="334"/>
+      <c r="L41" s="334"/>
       <c r="P41" s="268"/>
       <c r="Q41" s="268"/>
       <c r="R41" s="268"/>
@@ -44596,11 +44600,11 @@
       <c r="C42" s="268"/>
       <c r="D42" s="268"/>
       <c r="E42" s="268"/>
-      <c r="H42" s="343"/>
-      <c r="I42" s="343"/>
-      <c r="J42" s="343"/>
-      <c r="K42" s="343"/>
-      <c r="L42" s="343"/>
+      <c r="H42" s="334"/>
+      <c r="I42" s="334"/>
+      <c r="J42" s="334"/>
+      <c r="K42" s="334"/>
+      <c r="L42" s="334"/>
       <c r="P42" s="268"/>
       <c r="Q42" s="268"/>
       <c r="R42" s="268"/>
@@ -44618,11 +44622,11 @@
       <c r="C43" s="268"/>
       <c r="D43" s="268"/>
       <c r="E43" s="268"/>
-      <c r="H43" s="343"/>
-      <c r="I43" s="343"/>
-      <c r="J43" s="343"/>
-      <c r="K43" s="343"/>
-      <c r="L43" s="343"/>
+      <c r="H43" s="334"/>
+      <c r="I43" s="334"/>
+      <c r="J43" s="334"/>
+      <c r="K43" s="334"/>
+      <c r="L43" s="334"/>
       <c r="P43" s="268"/>
       <c r="Q43" s="268"/>
       <c r="R43" s="268"/>
@@ -44636,6 +44640,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A7:AA7"/>
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="F1:V4"/>
+    <mergeCell ref="W1:AA4"/>
+    <mergeCell ref="A5:W6"/>
+    <mergeCell ref="X5:AA6"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:S11"/>
     <mergeCell ref="AE12:AE13"/>
@@ -44643,12 +44653,6 @@
     <mergeCell ref="H40:L43"/>
     <mergeCell ref="P40:T43"/>
     <mergeCell ref="W40:AA43"/>
-    <mergeCell ref="A7:AA7"/>
-    <mergeCell ref="A1:E4"/>
-    <mergeCell ref="F1:V4"/>
-    <mergeCell ref="W1:AA4"/>
-    <mergeCell ref="A5:W6"/>
-    <mergeCell ref="X5:AA6"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -44670,215 +44674,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="334"/>
-      <c r="B1" s="334"/>
-      <c r="C1" s="334"/>
-      <c r="D1" s="334"/>
-      <c r="E1" s="334"/>
+      <c r="A1" s="339"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
       <c r="F1" s="311" t="s">
         <v>212</v>
       </c>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
-      <c r="P1" s="336"/>
-      <c r="Q1" s="336"/>
-      <c r="R1" s="336"/>
-      <c r="S1" s="336"/>
-      <c r="T1" s="336"/>
-      <c r="U1" s="336"/>
-      <c r="V1" s="336"/>
-      <c r="W1" s="334"/>
-      <c r="X1" s="334"/>
-      <c r="Y1" s="334"/>
-      <c r="Z1" s="334"/>
-      <c r="AA1" s="334"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="341"/>
+      <c r="I1" s="341"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="341"/>
+      <c r="L1" s="341"/>
+      <c r="M1" s="341"/>
+      <c r="N1" s="341"/>
+      <c r="O1" s="341"/>
+      <c r="P1" s="341"/>
+      <c r="Q1" s="341"/>
+      <c r="R1" s="341"/>
+      <c r="S1" s="341"/>
+      <c r="T1" s="341"/>
+      <c r="U1" s="341"/>
+      <c r="V1" s="341"/>
+      <c r="W1" s="339"/>
+      <c r="X1" s="339"/>
+      <c r="Y1" s="339"/>
+      <c r="Z1" s="339"/>
+      <c r="AA1" s="339"/>
     </row>
     <row r="2" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="334"/>
-      <c r="B2" s="334"/>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336"/>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336"/>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
-      <c r="T2" s="336"/>
-      <c r="U2" s="336"/>
-      <c r="V2" s="336"/>
-      <c r="W2" s="334"/>
-      <c r="X2" s="334"/>
-      <c r="Y2" s="334"/>
-      <c r="Z2" s="334"/>
-      <c r="AA2" s="334"/>
+      <c r="A2" s="339"/>
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
+      <c r="K2" s="341"/>
+      <c r="L2" s="341"/>
+      <c r="M2" s="341"/>
+      <c r="N2" s="341"/>
+      <c r="O2" s="341"/>
+      <c r="P2" s="341"/>
+      <c r="Q2" s="341"/>
+      <c r="R2" s="341"/>
+      <c r="S2" s="341"/>
+      <c r="T2" s="341"/>
+      <c r="U2" s="341"/>
+      <c r="V2" s="341"/>
+      <c r="W2" s="339"/>
+      <c r="X2" s="339"/>
+      <c r="Y2" s="339"/>
+      <c r="Z2" s="339"/>
+      <c r="AA2" s="339"/>
     </row>
     <row r="3" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="334"/>
-      <c r="B3" s="334"/>
-      <c r="C3" s="334"/>
-      <c r="D3" s="334"/>
-      <c r="E3" s="334"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
-      <c r="L3" s="336"/>
-      <c r="M3" s="336"/>
-      <c r="N3" s="336"/>
-      <c r="O3" s="336"/>
-      <c r="P3" s="336"/>
-      <c r="Q3" s="336"/>
-      <c r="R3" s="336"/>
-      <c r="S3" s="336"/>
-      <c r="T3" s="336"/>
-      <c r="U3" s="336"/>
-      <c r="V3" s="336"/>
-      <c r="W3" s="334"/>
-      <c r="X3" s="334"/>
-      <c r="Y3" s="334"/>
-      <c r="Z3" s="334"/>
-      <c r="AA3" s="334"/>
+      <c r="A3" s="339"/>
+      <c r="B3" s="339"/>
+      <c r="C3" s="339"/>
+      <c r="D3" s="339"/>
+      <c r="E3" s="339"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
+      <c r="K3" s="341"/>
+      <c r="L3" s="341"/>
+      <c r="M3" s="341"/>
+      <c r="N3" s="341"/>
+      <c r="O3" s="341"/>
+      <c r="P3" s="341"/>
+      <c r="Q3" s="341"/>
+      <c r="R3" s="341"/>
+      <c r="S3" s="341"/>
+      <c r="T3" s="341"/>
+      <c r="U3" s="341"/>
+      <c r="V3" s="341"/>
+      <c r="W3" s="339"/>
+      <c r="X3" s="339"/>
+      <c r="Y3" s="339"/>
+      <c r="Z3" s="339"/>
+      <c r="AA3" s="339"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="335"/>
-      <c r="B4" s="335"/>
-      <c r="C4" s="335"/>
-      <c r="D4" s="335"/>
-      <c r="E4" s="335"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="337"/>
-      <c r="L4" s="337"/>
-      <c r="M4" s="337"/>
-      <c r="N4" s="337"/>
-      <c r="O4" s="337"/>
-      <c r="P4" s="337"/>
-      <c r="Q4" s="337"/>
-      <c r="R4" s="337"/>
-      <c r="S4" s="337"/>
-      <c r="T4" s="337"/>
-      <c r="U4" s="337"/>
-      <c r="V4" s="337"/>
-      <c r="W4" s="335"/>
-      <c r="X4" s="335"/>
-      <c r="Y4" s="335"/>
-      <c r="Z4" s="335"/>
-      <c r="AA4" s="335"/>
+      <c r="A4" s="340"/>
+      <c r="B4" s="340"/>
+      <c r="C4" s="340"/>
+      <c r="D4" s="340"/>
+      <c r="E4" s="340"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="342"/>
+      <c r="M4" s="342"/>
+      <c r="N4" s="342"/>
+      <c r="O4" s="342"/>
+      <c r="P4" s="342"/>
+      <c r="Q4" s="342"/>
+      <c r="R4" s="342"/>
+      <c r="S4" s="342"/>
+      <c r="T4" s="342"/>
+      <c r="U4" s="342"/>
+      <c r="V4" s="342"/>
+      <c r="W4" s="340"/>
+      <c r="X4" s="340"/>
+      <c r="Y4" s="340"/>
+      <c r="Z4" s="340"/>
+      <c r="AA4" s="340"/>
     </row>
     <row r="5" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="338" t="s">
+      <c r="A5" s="343" t="s">
         <v>212</v>
       </c>
-      <c r="B5" s="338"/>
-      <c r="C5" s="338"/>
-      <c r="D5" s="338"/>
-      <c r="E5" s="338"/>
-      <c r="F5" s="338"/>
-      <c r="G5" s="338"/>
-      <c r="H5" s="338"/>
-      <c r="I5" s="338"/>
-      <c r="J5" s="338"/>
-      <c r="K5" s="338"/>
-      <c r="L5" s="338"/>
-      <c r="M5" s="338"/>
-      <c r="N5" s="338"/>
-      <c r="O5" s="338"/>
-      <c r="P5" s="338"/>
-      <c r="Q5" s="338"/>
-      <c r="R5" s="338"/>
-      <c r="S5" s="338"/>
-      <c r="T5" s="338"/>
-      <c r="U5" s="338"/>
-      <c r="V5" s="338"/>
-      <c r="W5" s="338"/>
-      <c r="X5" s="340" t="s">
+      <c r="B5" s="343"/>
+      <c r="C5" s="343"/>
+      <c r="D5" s="343"/>
+      <c r="E5" s="343"/>
+      <c r="F5" s="343"/>
+      <c r="G5" s="343"/>
+      <c r="H5" s="343"/>
+      <c r="I5" s="343"/>
+      <c r="J5" s="343"/>
+      <c r="K5" s="343"/>
+      <c r="L5" s="343"/>
+      <c r="M5" s="343"/>
+      <c r="N5" s="343"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="343"/>
+      <c r="Q5" s="343"/>
+      <c r="R5" s="343"/>
+      <c r="S5" s="343"/>
+      <c r="T5" s="343"/>
+      <c r="U5" s="343"/>
+      <c r="V5" s="343"/>
+      <c r="W5" s="343"/>
+      <c r="X5" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="340"/>
-      <c r="Z5" s="340"/>
-      <c r="AA5" s="340"/>
+      <c r="Y5" s="345"/>
+      <c r="Z5" s="345"/>
+      <c r="AA5" s="345"/>
     </row>
     <row r="6" spans="1:27" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="339"/>
-      <c r="B6" s="339"/>
-      <c r="C6" s="339"/>
-      <c r="D6" s="339"/>
-      <c r="E6" s="339"/>
-      <c r="F6" s="339"/>
-      <c r="G6" s="339"/>
-      <c r="H6" s="339"/>
-      <c r="I6" s="339"/>
-      <c r="J6" s="339"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="339"/>
-      <c r="M6" s="339"/>
-      <c r="N6" s="339"/>
-      <c r="O6" s="339"/>
-      <c r="P6" s="339"/>
-      <c r="Q6" s="339"/>
-      <c r="R6" s="339"/>
-      <c r="S6" s="339"/>
-      <c r="T6" s="339"/>
-      <c r="U6" s="339"/>
-      <c r="V6" s="339"/>
-      <c r="W6" s="339"/>
-      <c r="X6" s="341"/>
-      <c r="Y6" s="341"/>
-      <c r="Z6" s="341"/>
-      <c r="AA6" s="341"/>
+      <c r="A6" s="344"/>
+      <c r="B6" s="344"/>
+      <c r="C6" s="344"/>
+      <c r="D6" s="344"/>
+      <c r="E6" s="344"/>
+      <c r="F6" s="344"/>
+      <c r="G6" s="344"/>
+      <c r="H6" s="344"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
+      <c r="K6" s="344"/>
+      <c r="L6" s="344"/>
+      <c r="M6" s="344"/>
+      <c r="N6" s="344"/>
+      <c r="O6" s="344"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="344"/>
+      <c r="R6" s="344"/>
+      <c r="S6" s="344"/>
+      <c r="T6" s="344"/>
+      <c r="U6" s="344"/>
+      <c r="V6" s="344"/>
+      <c r="W6" s="344"/>
+      <c r="X6" s="346"/>
+      <c r="Y6" s="346"/>
+      <c r="Z6" s="346"/>
+      <c r="AA6" s="346"/>
     </row>
     <row r="7" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="300" t="s">
+      <c r="A7" s="296" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="300"/>
-      <c r="C7" s="300"/>
-      <c r="D7" s="300"/>
-      <c r="E7" s="300"/>
-      <c r="F7" s="300"/>
-      <c r="G7" s="300"/>
-      <c r="H7" s="300"/>
-      <c r="I7" s="300"/>
-      <c r="J7" s="300"/>
-      <c r="K7" s="300"/>
-      <c r="L7" s="300"/>
-      <c r="M7" s="300"/>
-      <c r="N7" s="300"/>
-      <c r="O7" s="300"/>
-      <c r="P7" s="300"/>
-      <c r="Q7" s="300"/>
-      <c r="R7" s="300"/>
-      <c r="S7" s="300"/>
-      <c r="T7" s="300"/>
-      <c r="U7" s="300"/>
-      <c r="V7" s="300"/>
-      <c r="W7" s="333"/>
-      <c r="X7" s="333"/>
-      <c r="Y7" s="333"/>
-      <c r="Z7" s="333"/>
-      <c r="AA7" s="333"/>
+      <c r="B7" s="296"/>
+      <c r="C7" s="296"/>
+      <c r="D7" s="296"/>
+      <c r="E7" s="296"/>
+      <c r="F7" s="296"/>
+      <c r="G7" s="296"/>
+      <c r="H7" s="296"/>
+      <c r="I7" s="296"/>
+      <c r="J7" s="296"/>
+      <c r="K7" s="296"/>
+      <c r="L7" s="296"/>
+      <c r="M7" s="296"/>
+      <c r="N7" s="296"/>
+      <c r="O7" s="296"/>
+      <c r="P7" s="296"/>
+      <c r="Q7" s="296"/>
+      <c r="R7" s="296"/>
+      <c r="S7" s="296"/>
+      <c r="T7" s="296"/>
+      <c r="U7" s="296"/>
+      <c r="V7" s="296"/>
+      <c r="W7" s="338"/>
+      <c r="X7" s="338"/>
+      <c r="Y7" s="338"/>
+      <c r="Z7" s="338"/>
+      <c r="AA7" s="338"/>
     </row>
     <row r="8" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="350" t="s">
@@ -46760,13 +46764,13 @@
       <c r="E40" s="280"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="342" t="s">
+      <c r="H40" s="333" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="342"/>
-      <c r="J40" s="342"/>
-      <c r="K40" s="342"/>
-      <c r="L40" s="342"/>
+      <c r="I40" s="333"/>
+      <c r="J40" s="333"/>
+      <c r="K40" s="333"/>
+      <c r="L40" s="333"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
@@ -46795,11 +46799,11 @@
       <c r="E41" s="268"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="343"/>
-      <c r="I41" s="343"/>
-      <c r="J41" s="343"/>
-      <c r="K41" s="343"/>
-      <c r="L41" s="343"/>
+      <c r="H41" s="334"/>
+      <c r="I41" s="334"/>
+      <c r="J41" s="334"/>
+      <c r="K41" s="334"/>
+      <c r="L41" s="334"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
@@ -46824,11 +46828,11 @@
       <c r="E42" s="268"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="343"/>
-      <c r="I42" s="343"/>
-      <c r="J42" s="343"/>
-      <c r="K42" s="343"/>
-      <c r="L42" s="343"/>
+      <c r="H42" s="334"/>
+      <c r="I42" s="334"/>
+      <c r="J42" s="334"/>
+      <c r="K42" s="334"/>
+      <c r="L42" s="334"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
@@ -46853,11 +46857,11 @@
       <c r="E43" s="268"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="343"/>
-      <c r="I43" s="343"/>
-      <c r="J43" s="343"/>
-      <c r="K43" s="343"/>
-      <c r="L43" s="343"/>
+      <c r="H43" s="334"/>
+      <c r="I43" s="334"/>
+      <c r="J43" s="334"/>
+      <c r="K43" s="334"/>
+      <c r="L43" s="334"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
@@ -46876,18 +46880,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:AA7"/>
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="F1:V4"/>
+    <mergeCell ref="W1:AA4"/>
+    <mergeCell ref="A5:W6"/>
+    <mergeCell ref="X5:AA6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A40:E43"/>
     <mergeCell ref="H40:L43"/>
     <mergeCell ref="P40:T43"/>
     <mergeCell ref="W40:AA43"/>
     <mergeCell ref="B8:V8"/>
-    <mergeCell ref="A7:AA7"/>
-    <mergeCell ref="A1:E4"/>
-    <mergeCell ref="F1:V4"/>
-    <mergeCell ref="W1:AA4"/>
-    <mergeCell ref="A5:W6"/>
-    <mergeCell ref="X5:AA6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -47043,11 +47047,11 @@
       <c r="Q5" s="217"/>
       <c r="S5" s="1"/>
       <c r="T5" s="66"/>
-      <c r="U5" s="360" t="s">
+      <c r="U5" s="355" t="s">
         <v>1</v>
       </c>
-      <c r="V5" s="360"/>
-      <c r="W5" s="360"/>
+      <c r="V5" s="355"/>
+      <c r="W5" s="355"/>
     </row>
     <row r="6" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -47071,35 +47075,35 @@
     </row>
     <row r="7" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="295" t="s">
+      <c r="B7" s="304" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="296"/>
-      <c r="D7" s="296"/>
-      <c r="E7" s="296"/>
-      <c r="F7" s="296"/>
-      <c r="G7" s="296"/>
-      <c r="H7" s="296"/>
-      <c r="I7" s="296"/>
-      <c r="J7" s="296"/>
-      <c r="K7" s="297"/>
+      <c r="C7" s="305"/>
+      <c r="D7" s="305"/>
+      <c r="E7" s="305"/>
+      <c r="F7" s="305"/>
+      <c r="G7" s="305"/>
+      <c r="H7" s="305"/>
+      <c r="I7" s="305"/>
+      <c r="J7" s="305"/>
+      <c r="K7" s="306"/>
       <c r="L7" s="217"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="295" t="s">
+      <c r="N7" s="304" t="s">
         <v>216</v>
       </c>
-      <c r="O7" s="296"/>
-      <c r="P7" s="296"/>
-      <c r="Q7" s="296"/>
-      <c r="R7" s="296"/>
-      <c r="S7" s="296"/>
-      <c r="T7" s="296"/>
-      <c r="U7" s="296"/>
-      <c r="V7" s="296"/>
-      <c r="W7" s="297"/>
+      <c r="O7" s="305"/>
+      <c r="P7" s="305"/>
+      <c r="Q7" s="305"/>
+      <c r="R7" s="305"/>
+      <c r="S7" s="305"/>
+      <c r="T7" s="305"/>
+      <c r="U7" s="305"/>
+      <c r="V7" s="305"/>
+      <c r="W7" s="306"/>
     </row>
     <row r="8" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="293" t="s">
+      <c r="A8" s="302" t="s">
         <v>217</v>
       </c>
       <c r="B8" s="315" t="s">
@@ -47115,23 +47119,23 @@
       <c r="J8" s="220"/>
       <c r="K8" s="220"/>
       <c r="L8" s="217"/>
-      <c r="M8" s="293" t="s">
+      <c r="M8" s="302" t="s">
         <v>217</v>
       </c>
-      <c r="N8" s="294" t="s">
+      <c r="N8" s="303" t="s">
         <v>218</v>
       </c>
-      <c r="O8" s="294"/>
-      <c r="P8" s="294"/>
-      <c r="Q8" s="294"/>
-      <c r="R8" s="294"/>
-      <c r="S8" s="294"/>
-      <c r="T8" s="294"/>
-      <c r="U8" s="294"/>
-      <c r="V8" s="294"/>
+      <c r="O8" s="303"/>
+      <c r="P8" s="303"/>
+      <c r="Q8" s="303"/>
+      <c r="R8" s="303"/>
+      <c r="S8" s="303"/>
+      <c r="T8" s="303"/>
+      <c r="U8" s="303"/>
+      <c r="V8" s="303"/>
     </row>
     <row r="9" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="293"/>
+      <c r="A9" s="302"/>
       <c r="B9" s="89"/>
       <c r="C9" s="90">
         <v>320</v>
@@ -47161,7 +47165,7 @@
         <v>960</v>
       </c>
       <c r="L9" s="217"/>
-      <c r="M9" s="293"/>
+      <c r="M9" s="302"/>
       <c r="N9" s="89"/>
       <c r="O9" s="90">
         <v>320</v>
@@ -47192,7 +47196,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="293"/>
+      <c r="A10" s="302"/>
       <c r="B10" s="222">
         <v>200</v>
       </c>
@@ -47224,7 +47228,7 @@
         <v>8613.5</v>
       </c>
       <c r="L10" s="217"/>
-      <c r="M10" s="293"/>
+      <c r="M10" s="302"/>
       <c r="N10" s="222">
         <v>200</v>
       </c>
@@ -47257,7 +47261,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="293"/>
+      <c r="A11" s="302"/>
       <c r="B11" s="222">
         <v>250</v>
       </c>
@@ -47289,7 +47293,7 @@
         <v>10010</v>
       </c>
       <c r="L11" s="217"/>
-      <c r="M11" s="293"/>
+      <c r="M11" s="302"/>
       <c r="N11" s="222">
         <v>250</v>
       </c>
@@ -47322,7 +47326,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="293"/>
+      <c r="A12" s="302"/>
       <c r="B12" s="222">
         <v>300</v>
       </c>
@@ -47354,7 +47358,7 @@
         <v>11410</v>
       </c>
       <c r="L12" s="217"/>
-      <c r="M12" s="293"/>
+      <c r="M12" s="302"/>
       <c r="N12" s="222">
         <v>300</v>
       </c>
@@ -47387,7 +47391,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="293"/>
+      <c r="A13" s="302"/>
       <c r="B13" s="222">
         <v>350</v>
       </c>
@@ -47419,7 +47423,7 @@
         <v>12806.5</v>
       </c>
       <c r="L13" s="217"/>
-      <c r="M13" s="293"/>
+      <c r="M13" s="302"/>
       <c r="N13" s="222">
         <v>350</v>
       </c>
@@ -47452,7 +47456,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="293"/>
+      <c r="A14" s="302"/>
       <c r="B14" s="222">
         <v>400</v>
       </c>
@@ -47484,7 +47488,7 @@
         <v>14598.5</v>
       </c>
       <c r="L14" s="217"/>
-      <c r="M14" s="293"/>
+      <c r="M14" s="302"/>
       <c r="N14" s="222">
         <v>400</v>
       </c>
@@ -47517,7 +47521,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="293"/>
+      <c r="A15" s="302"/>
       <c r="B15" s="222">
         <v>450</v>
       </c>
@@ -47549,7 +47553,7 @@
         <v>16005.5</v>
       </c>
       <c r="L15" s="217"/>
-      <c r="M15" s="293"/>
+      <c r="M15" s="302"/>
       <c r="N15" s="222">
         <v>450</v>
       </c>
@@ -47582,7 +47586,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="293"/>
+      <c r="A16" s="302"/>
       <c r="B16" s="222">
         <v>500</v>
       </c>
@@ -47614,7 +47618,7 @@
         <v>17412.5</v>
       </c>
       <c r="L16" s="217"/>
-      <c r="M16" s="293"/>
+      <c r="M16" s="302"/>
       <c r="N16" s="222">
         <v>500</v>
       </c>
@@ -47647,7 +47651,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="293"/>
+      <c r="A17" s="302"/>
       <c r="B17" s="222">
         <v>550</v>
       </c>
@@ -47679,7 +47683,7 @@
         <v>18819.5</v>
       </c>
       <c r="L17" s="217"/>
-      <c r="M17" s="293"/>
+      <c r="M17" s="302"/>
       <c r="N17" s="222">
         <v>550</v>
       </c>
@@ -47712,7 +47716,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="293"/>
+      <c r="A18" s="302"/>
       <c r="B18" s="222">
         <v>600</v>
       </c>
@@ -47744,7 +47748,7 @@
         <v>20510</v>
       </c>
       <c r="L18" s="217"/>
-      <c r="M18" s="293"/>
+      <c r="M18" s="302"/>
     </row>
     <row r="19" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -47759,13 +47763,13 @@
       <c r="J19" s="217"/>
       <c r="K19" s="217"/>
       <c r="L19" s="217"/>
-      <c r="M19" s="356" t="s">
+      <c r="M19" s="358" t="s">
         <v>75</v>
       </c>
-      <c r="N19" s="356"/>
-      <c r="O19" s="356"/>
-      <c r="P19" s="356"/>
-      <c r="Q19" s="356"/>
+      <c r="N19" s="358"/>
+      <c r="O19" s="358"/>
+      <c r="P19" s="358"/>
+      <c r="Q19" s="358"/>
       <c r="R19" s="112"/>
       <c r="S19" s="112"/>
       <c r="T19" s="112"/>
@@ -47774,18 +47778,18 @@
     </row>
     <row r="20" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="295" t="s">
+      <c r="B20" s="304" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="296"/>
-      <c r="D20" s="296"/>
-      <c r="E20" s="296"/>
-      <c r="F20" s="296"/>
-      <c r="G20" s="296"/>
-      <c r="H20" s="296"/>
-      <c r="I20" s="296"/>
-      <c r="J20" s="296"/>
-      <c r="K20" s="297"/>
+      <c r="C20" s="305"/>
+      <c r="D20" s="305"/>
+      <c r="E20" s="305"/>
+      <c r="F20" s="305"/>
+      <c r="G20" s="305"/>
+      <c r="H20" s="305"/>
+      <c r="I20" s="305"/>
+      <c r="J20" s="305"/>
+      <c r="K20" s="306"/>
       <c r="L20" s="217"/>
       <c r="M20" s="65"/>
       <c r="N20" s="228" t="s">
@@ -47805,7 +47809,7 @@
       <c r="Z20" s="228"/>
     </row>
     <row r="21" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="293" t="s">
+      <c r="A21" s="302" t="s">
         <v>221</v>
       </c>
       <c r="B21" s="315" t="s">
@@ -47836,7 +47840,7 @@
       <c r="W21" s="14"/>
     </row>
     <row r="22" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="293"/>
+      <c r="A22" s="302"/>
       <c r="B22" s="89"/>
       <c r="C22" s="90">
         <v>320</v>
@@ -47884,7 +47888,7 @@
       <c r="Z22" s="228"/>
     </row>
     <row r="23" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="293"/>
+      <c r="A23" s="302"/>
       <c r="B23" s="222">
         <v>200</v>
       </c>
@@ -47931,7 +47935,7 @@
       <c r="W23" s="228"/>
     </row>
     <row r="24" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="293"/>
+      <c r="A24" s="302"/>
       <c r="B24" s="222">
         <v>250</v>
       </c>
@@ -47977,7 +47981,7 @@
       <c r="V24" s="228"/>
     </row>
     <row r="25" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="293"/>
+      <c r="A25" s="302"/>
       <c r="B25" s="222">
         <v>300</v>
       </c>
@@ -48023,7 +48027,7 @@
       <c r="V25" s="228"/>
     </row>
     <row r="26" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="293"/>
+      <c r="A26" s="302"/>
       <c r="B26" s="222">
         <v>350</v>
       </c>
@@ -48069,7 +48073,7 @@
       <c r="V26" s="228"/>
     </row>
     <row r="27" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="293"/>
+      <c r="A27" s="302"/>
       <c r="B27" s="222">
         <v>400</v>
       </c>
@@ -48115,7 +48119,7 @@
       <c r="V27" s="228"/>
     </row>
     <row r="28" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="293"/>
+      <c r="A28" s="302"/>
       <c r="B28" s="222">
         <v>450</v>
       </c>
@@ -48161,7 +48165,7 @@
       <c r="V28" s="14"/>
     </row>
     <row r="29" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="293"/>
+      <c r="A29" s="302"/>
       <c r="B29" s="222">
         <v>500</v>
       </c>
@@ -48207,7 +48211,7 @@
       <c r="V29" s="228"/>
     </row>
     <row r="30" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="293"/>
+      <c r="A30" s="302"/>
       <c r="B30" s="222">
         <v>550</v>
       </c>
@@ -48253,7 +48257,7 @@
       <c r="V30" s="228"/>
     </row>
     <row r="31" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="293"/>
+      <c r="A31" s="302"/>
       <c r="B31" s="222">
         <v>600</v>
       </c>
@@ -48297,16 +48301,16 @@
       <c r="U31" s="228"/>
     </row>
     <row r="32" spans="1:26" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N32" s="355" t="s">
+      <c r="N32" s="357" t="s">
         <v>234</v>
       </c>
-      <c r="O32" s="355"/>
-      <c r="P32" s="355"/>
-      <c r="Q32" s="355"/>
-      <c r="R32" s="355"/>
-      <c r="S32" s="355"/>
-      <c r="T32" s="355"/>
-      <c r="U32" s="355"/>
+      <c r="O32" s="357"/>
+      <c r="P32" s="357"/>
+      <c r="Q32" s="357"/>
+      <c r="R32" s="357"/>
+      <c r="S32" s="357"/>
+      <c r="T32" s="357"/>
+      <c r="U32" s="357"/>
       <c r="V32" s="88"/>
       <c r="W32" s="88"/>
       <c r="X32" s="88"/>
@@ -48315,13 +48319,13 @@
     </row>
     <row r="33" spans="1:23" s="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="359" t="s">
+      <c r="A34" s="356" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="359"/>
-      <c r="C34" s="359"/>
-      <c r="D34" s="359"/>
-      <c r="E34" s="359"/>
+      <c r="B34" s="356"/>
+      <c r="C34" s="356"/>
+      <c r="D34" s="356"/>
+      <c r="E34" s="356"/>
       <c r="F34" s="268" t="s">
         <v>28</v>
       </c>
@@ -48331,21 +48335,21 @@
       <c r="J34" s="268"/>
       <c r="K34" s="214"/>
       <c r="L34" s="31"/>
-      <c r="M34" s="358" t="s">
+      <c r="M34" s="360" t="s">
         <v>29</v>
       </c>
-      <c r="N34" s="358"/>
-      <c r="O34" s="358"/>
-      <c r="P34" s="358"/>
-      <c r="Q34" s="358"/>
+      <c r="N34" s="360"/>
+      <c r="O34" s="360"/>
+      <c r="P34" s="360"/>
+      <c r="Q34" s="360"/>
       <c r="R34" s="31"/>
-      <c r="S34" s="357" t="s">
+      <c r="S34" s="359" t="s">
         <v>30</v>
       </c>
-      <c r="T34" s="357"/>
-      <c r="U34" s="357"/>
-      <c r="V34" s="357"/>
-      <c r="W34" s="357"/>
+      <c r="T34" s="359"/>
+      <c r="U34" s="359"/>
+      <c r="V34" s="359"/>
+      <c r="W34" s="359"/>
     </row>
     <row r="35" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="268"/>
@@ -48360,11 +48364,11 @@
       <c r="J35" s="268"/>
       <c r="K35" s="214"/>
       <c r="L35" s="31"/>
-      <c r="M35" s="358"/>
-      <c r="N35" s="358"/>
-      <c r="O35" s="358"/>
-      <c r="P35" s="358"/>
-      <c r="Q35" s="358"/>
+      <c r="M35" s="360"/>
+      <c r="N35" s="360"/>
+      <c r="O35" s="360"/>
+      <c r="P35" s="360"/>
+      <c r="Q35" s="360"/>
       <c r="R35" s="31"/>
       <c r="S35" s="270"/>
       <c r="T35" s="270"/>
@@ -48385,11 +48389,11 @@
       <c r="J36" s="268"/>
       <c r="K36" s="214"/>
       <c r="L36" s="31"/>
-      <c r="M36" s="358"/>
-      <c r="N36" s="358"/>
-      <c r="O36" s="358"/>
-      <c r="P36" s="358"/>
-      <c r="Q36" s="358"/>
+      <c r="M36" s="360"/>
+      <c r="N36" s="360"/>
+      <c r="O36" s="360"/>
+      <c r="P36" s="360"/>
+      <c r="Q36" s="360"/>
       <c r="R36" s="31"/>
       <c r="S36" s="270"/>
       <c r="T36" s="270"/>
@@ -48410,11 +48414,11 @@
       <c r="J37" s="268"/>
       <c r="K37" s="214"/>
       <c r="L37" s="31"/>
-      <c r="M37" s="358"/>
-      <c r="N37" s="358"/>
-      <c r="O37" s="358"/>
-      <c r="P37" s="358"/>
-      <c r="Q37" s="358"/>
+      <c r="M37" s="360"/>
+      <c r="N37" s="360"/>
+      <c r="O37" s="360"/>
+      <c r="P37" s="360"/>
+      <c r="Q37" s="360"/>
       <c r="R37" s="31"/>
       <c r="S37" s="270"/>
       <c r="T37" s="270"/>
@@ -48424,6 +48428,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N32:U32"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="S34:W37"/>
+    <mergeCell ref="M34:Q37"/>
+    <mergeCell ref="F34:J37"/>
+    <mergeCell ref="A34:E37"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="A21:A31"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="M8:M18"/>
     <mergeCell ref="U5:W5"/>
     <mergeCell ref="T1:W4"/>
@@ -48431,18 +48447,6 @@
     <mergeCell ref="N7:W7"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="N8:V8"/>
-    <mergeCell ref="A34:E37"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="A21:A31"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="N32:U32"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="S34:W37"/>
-    <mergeCell ref="M34:Q37"/>
-    <mergeCell ref="F34:J37"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0" top="0.39370078740157483" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>

</xml_diff>